<commit_message>
added weight interp, manually edited some weights
option added to main behavior file to interpolate weights between selected session #s

manually fixed some weights in the female early sessions (hadn't fixed them when I was editing them because they had the wrong subject labels).

edited tagnumber 38 too but unclear why it was so messed up. for some reason the weight was 0 for sessions 0, 1, 6, and 11. no idea how that happened.
</commit_message>
<xml_diff>
--- a/Outputs/Exp_all_Run_all_exclusions/Behavior Tables/run_all_exp_ER_GroupStats.xlsx
+++ b/Outputs/Exp_all_Run_all_exclusions/Behavior Tables/run_all_exp_ER_GroupStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="221" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1547" uniqueCount="22">
   <si>
     <t>Sex</t>
   </si>
@@ -1195,10 +1195,10 @@
         <v>124.50807692307683</v>
       </c>
       <c r="P20" s="0">
-        <v>59.720951008334417</v>
+        <v>59.82145489760461</v>
       </c>
       <c r="Q20" s="0">
-        <v>57.017462445790393</v>
+        <v>56.969700048919947</v>
       </c>
     </row>
     <row r="21">
@@ -2989,9 +2989,11 @@
         <v>83.158139318497049</v>
       </c>
       <c r="P54" s="0">
-        <v>65535</v>
-      </c>
-      <c r="Q54" s="0"/>
+        <v>56.220744202549618</v>
+      </c>
+      <c r="Q54" s="0">
+        <v>19.425478785356162</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="s">
@@ -3093,9 +3095,11 @@
         <v>320.97552634128039</v>
       </c>
       <c r="P56" s="0">
-        <v>65535</v>
-      </c>
-      <c r="Q56" s="0"/>
+        <v>114.90023813898675</v>
+      </c>
+      <c r="Q56" s="0">
+        <v>50.044468626942816</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="s">
@@ -3250,9 +3254,11 @@
         <v>158.54349546179873</v>
       </c>
       <c r="P59" s="0">
-        <v>65535</v>
-      </c>
-      <c r="Q59" s="0"/>
+        <v>61.087244108135195</v>
+      </c>
+      <c r="Q59" s="0">
+        <v>23.644092541978718</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="s">
@@ -3513,10 +3519,10 @@
         <v>1.8994763552843577</v>
       </c>
       <c r="P64" s="0">
-        <v>42.611982644485956</v>
+        <v>42.385652341041457</v>
       </c>
       <c r="Q64" s="0">
-        <v>9.8438187406455917</v>
+        <v>9.7041622791667983</v>
       </c>
     </row>
     <row r="65">
@@ -3566,9 +3572,11 @@
         <v>142.6828567917467</v>
       </c>
       <c r="P65" s="0">
-        <v>65535</v>
-      </c>
-      <c r="Q65" s="0"/>
+        <v>37.897737798460241</v>
+      </c>
+      <c r="Q65" s="0">
+        <v>17.144928103836946</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="s">

</xml_diff>

<commit_message>
missing session 19,20 data
added missing data from the 17th and 18th (sess 19 & 20).

minor bugfix in getFirstHour so it doesn't break for lack of 'Strain' column in our master sheet
</commit_message>
<xml_diff>
--- a/Outputs/Exp_all_Run_all_exclusions/Behavior Tables/run_all_exp_ER_GroupStats.xlsx
+++ b/Outputs/Exp_all_Run_all_exclusions/Behavior Tables/run_all_exp_ER_GroupStats.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="2922" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="3239" uniqueCount="22">
   <si>
     <t>Sex</t>
   </si>
@@ -124,7 +124,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q95"/>
+  <dimension ref="A1:Q101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1219,19 +1219,19 @@
         <v>19</v>
       </c>
       <c r="E21" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F21" s="0">
-        <v>2.5</v>
+        <v>12.75</v>
       </c>
       <c r="G21" s="0">
-        <v>0.5</v>
+        <v>7.1922991224410753</v>
       </c>
       <c r="H21" s="0">
-        <v>3.5</v>
+        <v>4.75</v>
       </c>
       <c r="I21" s="0">
-        <v>1.4999999999999998</v>
+        <v>1.25</v>
       </c>
       <c r="J21" s="0">
         <v>0</v>
@@ -1240,16 +1240,16 @@
         <v>0</v>
       </c>
       <c r="L21" s="0">
-        <v>7.5</v>
+        <v>22</v>
       </c>
       <c r="M21" s="0">
-        <v>2.5</v>
+        <v>9.65228815704684</v>
       </c>
       <c r="N21" s="0">
-        <v>381.89500000000004</v>
+        <v>336.57078571428571</v>
       </c>
       <c r="O21" s="0">
-        <v>214.03500000000003</v>
+        <v>105.10973618374919</v>
       </c>
       <c r="P21" s="0">
         <v>0</v>
@@ -1269,22 +1269,22 @@
         <v>6</v>
       </c>
       <c r="D22" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="0">
         <v>4</v>
       </c>
       <c r="F22" s="0">
-        <v>11.25</v>
+        <v>11.5</v>
       </c>
       <c r="G22" s="0">
-        <v>3.0652623596249202</v>
+        <v>4.1932485418030412</v>
       </c>
       <c r="H22" s="0">
-        <v>7</v>
+        <v>4.25</v>
       </c>
       <c r="I22" s="0">
-        <v>3.8514066694304478</v>
+        <v>2.0155644370746373</v>
       </c>
       <c r="J22" s="0">
         <v>0</v>
@@ -1293,16 +1293,16 @@
         <v>0</v>
       </c>
       <c r="L22" s="0">
-        <v>23</v>
+        <v>19.75</v>
       </c>
       <c r="M22" s="0">
-        <v>6.1237243569579451</v>
+        <v>5.2816506258302747</v>
       </c>
       <c r="N22" s="0">
-        <v>237.40952380952368</v>
+        <v>197.06520833333326</v>
       </c>
       <c r="O22" s="0">
-        <v>102.72177722002273</v>
+        <v>22.333011534723074</v>
       </c>
       <c r="P22" s="0">
         <v>0</v>
@@ -1322,22 +1322,22 @@
         <v>6</v>
       </c>
       <c r="D23" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E23" s="0">
         <v>4</v>
       </c>
       <c r="F23" s="0">
-        <v>10.25</v>
+        <v>11.25</v>
       </c>
       <c r="G23" s="0">
-        <v>3.9024564913226985</v>
+        <v>3.0652623596249202</v>
       </c>
       <c r="H23" s="0">
-        <v>5.75</v>
+        <v>7</v>
       </c>
       <c r="I23" s="0">
-        <v>3.0652623596249202</v>
+        <v>3.8514066694304478</v>
       </c>
       <c r="J23" s="0">
         <v>0</v>
@@ -1346,16 +1346,16 @@
         <v>0</v>
       </c>
       <c r="L23" s="0">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="M23" s="0">
-        <v>13.946325680981353</v>
+        <v>6.1237243569579451</v>
       </c>
       <c r="N23" s="0">
-        <v>155.78484126984128</v>
+        <v>237.40952380952368</v>
       </c>
       <c r="O23" s="0">
-        <v>31.833919123652151</v>
+        <v>102.72177722002273</v>
       </c>
       <c r="P23" s="0">
         <v>0</v>
@@ -1375,22 +1375,22 @@
         <v>6</v>
       </c>
       <c r="D24" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E24" s="0">
         <v>4</v>
       </c>
       <c r="F24" s="0">
-        <v>16</v>
+        <v>10.25</v>
       </c>
       <c r="G24" s="0">
-        <v>8.1342895612749526</v>
+        <v>3.9024564913226985</v>
       </c>
       <c r="H24" s="0">
-        <v>3.75</v>
+        <v>5.75</v>
       </c>
       <c r="I24" s="0">
-        <v>1.8874586088176875</v>
+        <v>3.0652623596249202</v>
       </c>
       <c r="J24" s="0">
         <v>0</v>
@@ -1399,16 +1399,16 @@
         <v>0</v>
       </c>
       <c r="L24" s="0">
-        <v>25.5</v>
+        <v>40</v>
       </c>
       <c r="M24" s="0">
-        <v>8.9116029235298999</v>
+        <v>13.946325680981353</v>
       </c>
       <c r="N24" s="0">
-        <v>327.49862499999983</v>
+        <v>155.78484126984128</v>
       </c>
       <c r="O24" s="0">
-        <v>211.12187136870489</v>
+        <v>31.833919123652151</v>
       </c>
       <c r="P24" s="0">
         <v>0</v>
@@ -1428,40 +1428,40 @@
         <v>6</v>
       </c>
       <c r="D25" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E25" s="0">
         <v>4</v>
       </c>
       <c r="F25" s="0">
-        <v>18.75</v>
+        <v>16</v>
       </c>
       <c r="G25" s="0">
-        <v>4.3851073723076235</v>
+        <v>8.1342895612749526</v>
       </c>
       <c r="H25" s="0">
-        <v>1.25</v>
+        <v>3.75</v>
       </c>
       <c r="I25" s="0">
-        <v>0.62915286960589578</v>
+        <v>1.8874586088176875</v>
       </c>
       <c r="J25" s="0">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="K25" s="0">
-        <v>3.3911649915626341</v>
+        <v>0</v>
       </c>
       <c r="L25" s="0">
-        <v>15</v>
+        <v>25.5</v>
       </c>
       <c r="M25" s="0">
-        <v>6.6833125519211407</v>
+        <v>8.9116029235298999</v>
       </c>
       <c r="N25" s="0">
-        <v>231.06038461538463</v>
+        <v>327.49862499999983</v>
       </c>
       <c r="O25" s="0">
-        <v>172.66941114087831</v>
+        <v>211.12187136870489</v>
       </c>
       <c r="P25" s="0">
         <v>0</v>
@@ -1478,40 +1478,44 @@
         <v>4</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D26" s="0">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E26" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F26" s="0">
-        <v>22.333333333333332</v>
+        <v>18.75</v>
       </c>
       <c r="G26" s="0">
-        <v>5.8404718226450774</v>
+        <v>4.3851073723076235</v>
       </c>
       <c r="H26" s="0">
-        <v>11.333333333333334</v>
+        <v>1.25</v>
       </c>
       <c r="I26" s="0">
-        <v>2.9059326290271157</v>
+        <v>0.62915286960589578</v>
       </c>
       <c r="J26" s="0">
         <v>11</v>
       </c>
       <c r="K26" s="0">
-        <v>0.57735026918962584</v>
+        <v>3.3911649915626341</v>
       </c>
       <c r="L26" s="0">
-        <v>42.666666666666664</v>
+        <v>15</v>
       </c>
       <c r="M26" s="0">
-        <v>13.245544324203685</v>
-      </c>
-      <c r="N26" s="0"/>
-      <c r="O26" s="0"/>
+        <v>6.6833125519211407</v>
+      </c>
+      <c r="N26" s="0">
+        <v>231.06038461538463</v>
+      </c>
+      <c r="O26" s="0">
+        <v>172.66941114087831</v>
+      </c>
       <c r="P26" s="0">
         <v>0</v>
       </c>
@@ -1530,46 +1534,42 @@
         <v>7</v>
       </c>
       <c r="D27" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="0">
         <v>3</v>
       </c>
       <c r="F27" s="0">
-        <v>17.666666666666668</v>
+        <v>22.333333333333332</v>
       </c>
       <c r="G27" s="0">
-        <v>17.169093679567879</v>
+        <v>5.8404718226450774</v>
       </c>
       <c r="H27" s="0">
-        <v>0.33333333333333331</v>
+        <v>11.333333333333334</v>
       </c>
       <c r="I27" s="0">
-        <v>0.33333333333333337</v>
+        <v>2.9059326290271157</v>
       </c>
       <c r="J27" s="0">
         <v>11</v>
       </c>
       <c r="K27" s="0">
-        <v>10.503967504392488</v>
+        <v>0.57735026918962584</v>
       </c>
       <c r="L27" s="0">
-        <v>66</v>
+        <v>42.666666666666664</v>
       </c>
       <c r="M27" s="0">
-        <v>23.797758998135379</v>
-      </c>
-      <c r="N27" s="0">
-        <v>147.12807692307683</v>
-      </c>
-      <c r="O27" s="0">
-        <v>124.50807692307683</v>
-      </c>
+        <v>13.245544324203685</v>
+      </c>
+      <c r="N27" s="0"/>
+      <c r="O27" s="0"/>
       <c r="P27" s="0">
-        <v>59.82145489760461</v>
+        <v>0</v>
       </c>
       <c r="Q27" s="0">
-        <v>56.969700048919947</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1583,46 +1583,46 @@
         <v>7</v>
       </c>
       <c r="D28" s="0">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="0">
         <v>3</v>
       </c>
       <c r="F28" s="0">
-        <v>15.666666666666666</v>
+        <v>17.666666666666668</v>
       </c>
       <c r="G28" s="0">
-        <v>7.4236858171066959</v>
+        <v>17.169093679567879</v>
       </c>
       <c r="H28" s="0">
-        <v>6.666666666666667</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="I28" s="0">
-        <v>6.666666666666667</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="J28" s="0">
-        <v>9.6666666666666661</v>
+        <v>11</v>
       </c>
       <c r="K28" s="0">
-        <v>4.4845413490245702</v>
+        <v>10.503967504392488</v>
       </c>
       <c r="L28" s="0">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M28" s="0">
-        <v>15.176736583776281</v>
+        <v>23.797758998135379</v>
       </c>
       <c r="N28" s="0">
-        <v>50.378703703703508</v>
+        <v>147.12807692307683</v>
       </c>
       <c r="O28" s="0">
-        <v>27.410077455651834</v>
+        <v>124.50807692307683</v>
       </c>
       <c r="P28" s="0">
-        <v>56.2978047256697</v>
+        <v>59.82145489760461</v>
       </c>
       <c r="Q28" s="0">
-        <v>26.47196134009884</v>
+        <v>56.969700048919947</v>
       </c>
     </row>
     <row r="29">
@@ -1636,46 +1636,46 @@
         <v>7</v>
       </c>
       <c r="D29" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" s="0">
         <v>3</v>
       </c>
       <c r="F29" s="0">
-        <v>36.666666666666664</v>
+        <v>15.666666666666666</v>
       </c>
       <c r="G29" s="0">
-        <v>9.0615181460454579</v>
+        <v>7.4236858171066959</v>
       </c>
       <c r="H29" s="0">
-        <v>8.3333333333333339</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="I29" s="0">
-        <v>6.8879927732572757</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="J29" s="0">
-        <v>23.333333333333332</v>
+        <v>9.6666666666666661</v>
       </c>
       <c r="K29" s="0">
-        <v>6.1734197258173786</v>
+        <v>4.4845413490245702</v>
       </c>
       <c r="L29" s="0">
-        <v>37.333333333333336</v>
+        <v>62</v>
       </c>
       <c r="M29" s="0">
-        <v>18.351506144667738</v>
+        <v>15.176736583776281</v>
       </c>
       <c r="N29" s="0">
-        <v>171.12352130325806</v>
+        <v>50.378703703703508</v>
       </c>
       <c r="O29" s="0">
-        <v>92.757489371524173</v>
+        <v>27.410077455651834</v>
       </c>
       <c r="P29" s="0">
-        <v>131.14162865217881</v>
+        <v>56.2978047256697</v>
       </c>
       <c r="Q29" s="0">
-        <v>31.421736740495735</v>
+        <v>26.47196134009884</v>
       </c>
     </row>
     <row r="30">
@@ -1689,46 +1689,46 @@
         <v>7</v>
       </c>
       <c r="D30" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E30" s="0">
         <v>3</v>
       </c>
       <c r="F30" s="0">
-        <v>62.333333333333336</v>
+        <v>36.666666666666664</v>
       </c>
       <c r="G30" s="0">
-        <v>41.929835572192637</v>
+        <v>9.0615181460454579</v>
       </c>
       <c r="H30" s="0">
-        <v>4.333333333333333</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="I30" s="0">
-        <v>3.3829638550307402</v>
+        <v>6.8879927732572757</v>
       </c>
       <c r="J30" s="0">
-        <v>33.333333333333336</v>
+        <v>23.333333333333332</v>
       </c>
       <c r="K30" s="0">
-        <v>18.835545592782221</v>
+        <v>6.1734197258173786</v>
       </c>
       <c r="L30" s="0">
-        <v>25.666666666666668</v>
+        <v>37.333333333333336</v>
       </c>
       <c r="M30" s="0">
-        <v>9.207484877955423</v>
+        <v>18.351506144667738</v>
       </c>
       <c r="N30" s="0">
-        <v>154.30480341880343</v>
+        <v>171.12352130325806</v>
       </c>
       <c r="O30" s="0">
-        <v>34.836998057684639</v>
+        <v>92.757489371524173</v>
       </c>
       <c r="P30" s="0">
-        <v>184.54345251674729</v>
+        <v>131.14162865217881</v>
       </c>
       <c r="Q30" s="0">
-        <v>101.13365237041019</v>
+        <v>31.421736740495735</v>
       </c>
     </row>
     <row r="31">
@@ -1742,46 +1742,46 @@
         <v>7</v>
       </c>
       <c r="D31" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E31" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F31" s="0">
-        <v>12</v>
+        <v>62.333333333333336</v>
       </c>
       <c r="G31" s="0">
-        <v>0</v>
+        <v>41.929835572192637</v>
       </c>
       <c r="H31" s="0">
-        <v>0</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="I31" s="0">
-        <v>0</v>
+        <v>3.3829638550307402</v>
       </c>
       <c r="J31" s="0">
-        <v>9</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="K31" s="0">
-        <v>0</v>
+        <v>18.835545592782221</v>
       </c>
       <c r="L31" s="0">
-        <v>55</v>
+        <v>25.666666666666668</v>
       </c>
       <c r="M31" s="0">
-        <v>0</v>
+        <v>9.207484877955423</v>
       </c>
       <c r="N31" s="0">
-        <v>315.25999999999999</v>
+        <v>154.30480341880343</v>
       </c>
       <c r="O31" s="0">
-        <v>0</v>
+        <v>34.836998057684639</v>
       </c>
       <c r="P31" s="0">
-        <v>51.767234042553206</v>
+        <v>184.54345251674729</v>
       </c>
       <c r="Q31" s="0">
-        <v>0</v>
+        <v>101.13365237041019</v>
       </c>
     </row>
     <row r="32">
@@ -1795,46 +1795,46 @@
         <v>7</v>
       </c>
       <c r="D32" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E32" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F32" s="0">
-        <v>39.333333333333336</v>
+        <v>12</v>
       </c>
       <c r="G32" s="0">
-        <v>13.017082793177757</v>
+        <v>0</v>
       </c>
       <c r="H32" s="0">
-        <v>11.333333333333334</v>
+        <v>0</v>
       </c>
       <c r="I32" s="0">
-        <v>10.333333333333334</v>
+        <v>0</v>
       </c>
       <c r="J32" s="0">
-        <v>24.666666666666668</v>
+        <v>9</v>
       </c>
       <c r="K32" s="0">
-        <v>8.6666666666666679</v>
+        <v>0</v>
       </c>
       <c r="L32" s="0">
-        <v>38.666666666666664</v>
+        <v>55</v>
       </c>
       <c r="M32" s="0">
-        <v>1.2018504251546631</v>
+        <v>0</v>
       </c>
       <c r="N32" s="0">
-        <v>193.94226190476198</v>
+        <v>315.25999999999999</v>
       </c>
       <c r="O32" s="0">
-        <v>64.546990462261391</v>
+        <v>0</v>
       </c>
       <c r="P32" s="0">
-        <v>135.36147039755053</v>
+        <v>51.767234042553206</v>
       </c>
       <c r="Q32" s="0">
-        <v>47.607984224371108</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1848,46 +1848,46 @@
         <v>7</v>
       </c>
       <c r="D33" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E33" s="0">
         <v>3</v>
       </c>
       <c r="F33" s="0">
-        <v>20.666666666666668</v>
+        <v>39.333333333333336</v>
       </c>
       <c r="G33" s="0">
-        <v>7.2188026092359054</v>
+        <v>13.017082793177757</v>
       </c>
       <c r="H33" s="0">
-        <v>2.3333333333333335</v>
+        <v>11.333333333333334</v>
       </c>
       <c r="I33" s="0">
-        <v>1.8559214542766742</v>
+        <v>10.333333333333334</v>
       </c>
       <c r="J33" s="0">
-        <v>16</v>
+        <v>24.666666666666668</v>
       </c>
       <c r="K33" s="0">
-        <v>3.2145502536643185</v>
+        <v>8.6666666666666679</v>
       </c>
       <c r="L33" s="0">
-        <v>28.333333333333332</v>
+        <v>38.666666666666664</v>
       </c>
       <c r="M33" s="0">
-        <v>15.719768163402129</v>
+        <v>1.2018504251546631</v>
       </c>
       <c r="N33" s="0">
-        <v>141.20233333333331</v>
+        <v>193.94226190476198</v>
       </c>
       <c r="O33" s="0">
-        <v>26.809651749433957</v>
+        <v>64.546990462261391</v>
       </c>
       <c r="P33" s="0">
-        <v>89.13695704326004</v>
+        <v>135.36147039755053</v>
       </c>
       <c r="Q33" s="0">
-        <v>19.774548598661202</v>
+        <v>47.607984224371108</v>
       </c>
     </row>
     <row r="34">
@@ -1901,46 +1901,46 @@
         <v>7</v>
       </c>
       <c r="D34" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E34" s="0">
         <v>3</v>
       </c>
       <c r="F34" s="0">
-        <v>26.666666666666668</v>
+        <v>20.666666666666668</v>
       </c>
       <c r="G34" s="0">
-        <v>9.9554563487120529</v>
+        <v>7.2188026092359054</v>
       </c>
       <c r="H34" s="0">
-        <v>4.666666666666667</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="I34" s="0">
-        <v>4.1766546953805559</v>
+        <v>1.8559214542766742</v>
       </c>
       <c r="J34" s="0">
-        <v>19.333333333333332</v>
+        <v>16</v>
       </c>
       <c r="K34" s="0">
-        <v>5.7831171909658243</v>
+        <v>3.2145502536643185</v>
       </c>
       <c r="L34" s="0">
-        <v>34.666666666666664</v>
+        <v>28.333333333333332</v>
       </c>
       <c r="M34" s="0">
-        <v>11.89304184994085</v>
+        <v>15.719768163402129</v>
       </c>
       <c r="N34" s="0">
-        <v>103.55441798941801</v>
+        <v>141.20233333333331</v>
       </c>
       <c r="O34" s="0">
-        <v>31.842857207617705</v>
+        <v>26.809651749433957</v>
       </c>
       <c r="P34" s="0">
-        <v>108.15475427996523</v>
+        <v>89.13695704326004</v>
       </c>
       <c r="Q34" s="0">
-        <v>33.800915352693998</v>
+        <v>19.774548598661202</v>
       </c>
     </row>
     <row r="35">
@@ -1954,46 +1954,46 @@
         <v>7</v>
       </c>
       <c r="D35" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E35" s="0">
         <v>3</v>
       </c>
       <c r="F35" s="0">
-        <v>14.666666666666666</v>
+        <v>26.666666666666668</v>
       </c>
       <c r="G35" s="0">
-        <v>2.728450923957483</v>
+        <v>9.9554563487120529</v>
       </c>
       <c r="H35" s="0">
-        <v>6.333333333333333</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="I35" s="0">
-        <v>3.2829526005987018</v>
+        <v>4.1766546953805559</v>
       </c>
       <c r="J35" s="0">
-        <v>12.333333333333334</v>
+        <v>19.333333333333332</v>
       </c>
       <c r="K35" s="0">
-        <v>2.8480012484391777</v>
+        <v>5.7831171909658243</v>
       </c>
       <c r="L35" s="0">
-        <v>24.333333333333332</v>
+        <v>34.666666666666664</v>
       </c>
       <c r="M35" s="0">
-        <v>9.4044906531105923</v>
+        <v>11.89304184994085</v>
       </c>
       <c r="N35" s="0">
-        <v>259.80317460317463</v>
+        <v>103.55441798941801</v>
       </c>
       <c r="O35" s="0">
-        <v>181.81741983243114</v>
+        <v>31.842857207617705</v>
       </c>
       <c r="P35" s="0">
-        <v>67.453179995532537</v>
+        <v>108.15475427996523</v>
       </c>
       <c r="Q35" s="0">
-        <v>14.024567676957011</v>
+        <v>33.800915352693998</v>
       </c>
     </row>
     <row r="36">
@@ -2007,46 +2007,46 @@
         <v>7</v>
       </c>
       <c r="D36" s="0">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E36" s="0">
         <v>3</v>
       </c>
       <c r="F36" s="0">
-        <v>10.333333333333334</v>
+        <v>14.666666666666666</v>
       </c>
       <c r="G36" s="0">
-        <v>2.3333333333333335</v>
+        <v>2.728450923957483</v>
       </c>
       <c r="H36" s="0">
-        <v>1.3333333333333333</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="I36" s="0">
-        <v>0.88191710368819698</v>
+        <v>3.2829526005987018</v>
       </c>
       <c r="J36" s="0">
-        <v>9</v>
+        <v>12.333333333333334</v>
       </c>
       <c r="K36" s="0">
-        <v>1</v>
+        <v>2.8480012484391777</v>
       </c>
       <c r="L36" s="0">
-        <v>35.333333333333336</v>
+        <v>24.333333333333332</v>
       </c>
       <c r="M36" s="0">
-        <v>14.847371634213394</v>
+        <v>9.4044906531105923</v>
       </c>
       <c r="N36" s="0">
-        <v>187.92211640211642</v>
+        <v>259.80317460317463</v>
       </c>
       <c r="O36" s="0">
-        <v>107.7609416840225</v>
+        <v>181.81741983243114</v>
       </c>
       <c r="P36" s="0">
-        <v>49.909091132794707</v>
+        <v>67.453179995532537</v>
       </c>
       <c r="Q36" s="0">
-        <v>6.5701566750317086</v>
+        <v>14.024567676957011</v>
       </c>
     </row>
     <row r="37">
@@ -2060,46 +2060,46 @@
         <v>7</v>
       </c>
       <c r="D37" s="0">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E37" s="0">
         <v>3</v>
       </c>
       <c r="F37" s="0">
-        <v>54.333333333333336</v>
+        <v>10.333333333333334</v>
       </c>
       <c r="G37" s="0">
-        <v>5.0442486501405197</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="H37" s="0">
-        <v>7.666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="I37" s="0">
-        <v>3.2829526005987018</v>
+        <v>0.88191710368819698</v>
       </c>
       <c r="J37" s="0">
-        <v>38.333333333333336</v>
+        <v>9</v>
       </c>
       <c r="K37" s="0">
-        <v>3.8441875315569325</v>
+        <v>1</v>
       </c>
       <c r="L37" s="0">
-        <v>40.333333333333336</v>
+        <v>35.333333333333336</v>
       </c>
       <c r="M37" s="0">
-        <v>16.333333333333332</v>
+        <v>14.847371634213394</v>
       </c>
       <c r="N37" s="0">
-        <v>242.66604797979792</v>
+        <v>187.92211640211642</v>
       </c>
       <c r="O37" s="0">
-        <v>85.094911956049671</v>
+        <v>107.7609416840225</v>
       </c>
       <c r="P37" s="0">
-        <v>208.23127448771447</v>
+        <v>49.909091132794707</v>
       </c>
       <c r="Q37" s="0">
-        <v>23.504791614783297</v>
+        <v>6.5701566750317086</v>
       </c>
     </row>
     <row r="38">
@@ -2113,46 +2113,46 @@
         <v>7</v>
       </c>
       <c r="D38" s="0">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E38" s="0">
         <v>3</v>
       </c>
       <c r="F38" s="0">
-        <v>29.333333333333332</v>
+        <v>54.333333333333336</v>
       </c>
       <c r="G38" s="0">
-        <v>8.192137151629673</v>
+        <v>5.0442486501405197</v>
       </c>
       <c r="H38" s="0">
-        <v>5.666666666666667</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="I38" s="0">
-        <v>3.4801021696368499</v>
+        <v>3.2829526005987018</v>
       </c>
       <c r="J38" s="0">
-        <v>20</v>
+        <v>38.333333333333336</v>
       </c>
       <c r="K38" s="0">
-        <v>4.1633319989322652</v>
+        <v>3.8441875315569325</v>
       </c>
       <c r="L38" s="0">
-        <v>20.666666666666668</v>
+        <v>40.333333333333336</v>
       </c>
       <c r="M38" s="0">
-        <v>5.9254629448770597</v>
+        <v>16.333333333333332</v>
       </c>
       <c r="N38" s="0">
-        <v>475.97514814814809</v>
+        <v>242.66604797979792</v>
       </c>
       <c r="O38" s="0">
-        <v>189.44740330327915</v>
+        <v>85.094911956049671</v>
       </c>
       <c r="P38" s="0">
-        <v>107.74190013548792</v>
+        <v>208.23127448771447</v>
       </c>
       <c r="Q38" s="0">
-        <v>21.020762780909553</v>
+        <v>23.504791614783297</v>
       </c>
     </row>
     <row r="39">
@@ -2166,46 +2166,46 @@
         <v>7</v>
       </c>
       <c r="D39" s="0">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E39" s="0">
         <v>3</v>
       </c>
       <c r="F39" s="0">
-        <v>37.666666666666664</v>
+        <v>29.333333333333332</v>
       </c>
       <c r="G39" s="0">
-        <v>8.6666666666666679</v>
+        <v>8.192137151629673</v>
       </c>
       <c r="H39" s="0">
-        <v>12.666666666666666</v>
+        <v>5.666666666666667</v>
       </c>
       <c r="I39" s="0">
-        <v>5.3644923131436943</v>
+        <v>3.4801021696368499</v>
       </c>
       <c r="J39" s="0">
-        <v>26.333333333333332</v>
+        <v>20</v>
       </c>
       <c r="K39" s="0">
-        <v>6.8394281762277309</v>
+        <v>4.1633319989322652</v>
       </c>
       <c r="L39" s="0">
-        <v>33.333333333333336</v>
+        <v>20.666666666666668</v>
       </c>
       <c r="M39" s="0">
-        <v>4.1766546953805559</v>
+        <v>5.9254629448770597</v>
       </c>
       <c r="N39" s="0">
-        <v>304.37674857549854</v>
+        <v>475.97514814814809</v>
       </c>
       <c r="O39" s="0">
-        <v>157.7987128212724</v>
+        <v>189.44740330327915</v>
       </c>
       <c r="P39" s="0">
-        <v>143.33137566805161</v>
+        <v>107.74190013548792</v>
       </c>
       <c r="Q39" s="0">
-        <v>38.686492556508803</v>
+        <v>21.020762780909553</v>
       </c>
     </row>
     <row r="40">
@@ -2219,46 +2219,46 @@
         <v>7</v>
       </c>
       <c r="D40" s="0">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E40" s="0">
         <v>3</v>
       </c>
       <c r="F40" s="0">
-        <v>17</v>
+        <v>37.666666666666664</v>
       </c>
       <c r="G40" s="0">
-        <v>5.2915026221291814</v>
+        <v>8.6666666666666679</v>
       </c>
       <c r="H40" s="0">
-        <v>4.333333333333333</v>
+        <v>12.666666666666666</v>
       </c>
       <c r="I40" s="0">
-        <v>4.3333333333333339</v>
+        <v>5.3644923131436943</v>
       </c>
       <c r="J40" s="0">
-        <v>13.666666666666666</v>
+        <v>26.333333333333332</v>
       </c>
       <c r="K40" s="0">
-        <v>3.7564758898615485</v>
+        <v>6.8394281762277309</v>
       </c>
       <c r="L40" s="0">
-        <v>19.666666666666668</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="M40" s="0">
-        <v>9.5277372853043012</v>
+        <v>4.1766546953805559</v>
       </c>
       <c r="N40" s="0">
-        <v>375.290202020202</v>
+        <v>304.37674857549854</v>
       </c>
       <c r="O40" s="0">
-        <v>169.71056913701193</v>
+        <v>157.7987128212724</v>
       </c>
       <c r="P40" s="0">
-        <v>74.186329358820686</v>
+        <v>143.33137566805161</v>
       </c>
       <c r="Q40" s="0">
-        <v>21.122182496662028</v>
+        <v>38.686492556508803</v>
       </c>
     </row>
     <row r="41">
@@ -2272,46 +2272,46 @@
         <v>7</v>
       </c>
       <c r="D41" s="0">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E41" s="0">
         <v>3</v>
       </c>
       <c r="F41" s="0">
-        <v>26.666666666666668</v>
+        <v>17</v>
       </c>
       <c r="G41" s="0">
-        <v>12.719189352225943</v>
+        <v>5.2915026221291814</v>
       </c>
       <c r="H41" s="0">
-        <v>4.666666666666667</v>
+        <v>4.333333333333333</v>
       </c>
       <c r="I41" s="0">
-        <v>1.4529663145135578</v>
+        <v>4.3333333333333339</v>
       </c>
       <c r="J41" s="0">
+        <v>13.666666666666666</v>
+      </c>
+      <c r="K41" s="0">
+        <v>3.7564758898615485</v>
+      </c>
+      <c r="L41" s="0">
         <v>19.666666666666668</v>
       </c>
-      <c r="K41" s="0">
-        <v>8.6666666666666679</v>
-      </c>
-      <c r="L41" s="0">
-        <v>29.333333333333332</v>
-      </c>
       <c r="M41" s="0">
-        <v>15.835964693626272</v>
+        <v>9.5277372853043012</v>
       </c>
       <c r="N41" s="0">
-        <v>313.52541666666667</v>
+        <v>375.290202020202</v>
       </c>
       <c r="O41" s="0">
-        <v>156.1473641513798</v>
+        <v>169.71056913701193</v>
       </c>
       <c r="P41" s="0">
-        <v>104.33947060573014</v>
+        <v>74.186329358820686</v>
       </c>
       <c r="Q41" s="0">
-        <v>43.275275321843061</v>
+        <v>21.122182496662028</v>
       </c>
     </row>
     <row r="42">
@@ -2325,46 +2325,46 @@
         <v>7</v>
       </c>
       <c r="D42" s="0">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E42" s="0">
         <v>3</v>
       </c>
       <c r="F42" s="0">
-        <v>29.666666666666668</v>
+        <v>26.666666666666668</v>
       </c>
       <c r="G42" s="0">
-        <v>3.5276684147527875</v>
+        <v>12.719189352225943</v>
       </c>
       <c r="H42" s="0">
-        <v>6.666666666666667</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="I42" s="0">
-        <v>2.6034165586355518</v>
+        <v>1.4529663145135578</v>
       </c>
       <c r="J42" s="0">
-        <v>0</v>
+        <v>19.666666666666668</v>
       </c>
       <c r="K42" s="0">
-        <v>0</v>
+        <v>8.6666666666666679</v>
       </c>
       <c r="L42" s="0">
-        <v>32.666666666666664</v>
+        <v>29.333333333333332</v>
       </c>
       <c r="M42" s="0">
-        <v>8.3732377913869804</v>
+        <v>15.835964693626272</v>
       </c>
       <c r="N42" s="0">
-        <v>152.85188888888891</v>
+        <v>313.52541666666667</v>
       </c>
       <c r="O42" s="0">
-        <v>59.54986197214258</v>
+        <v>156.1473641513798</v>
       </c>
       <c r="P42" s="0">
-        <v>0</v>
+        <v>104.33947060573014</v>
       </c>
       <c r="Q42" s="0">
-        <v>0</v>
+        <v>43.275275321843061</v>
       </c>
     </row>
     <row r="43">
@@ -2378,22 +2378,22 @@
         <v>7</v>
       </c>
       <c r="D43" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E43" s="0">
         <v>3</v>
       </c>
       <c r="F43" s="0">
-        <v>16</v>
+        <v>29.666666666666668</v>
       </c>
       <c r="G43" s="0">
-        <v>4</v>
+        <v>3.5276684147527875</v>
       </c>
       <c r="H43" s="0">
-        <v>9.6666666666666661</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="I43" s="0">
-        <v>3.3333333333333335</v>
+        <v>2.6034165586355518</v>
       </c>
       <c r="J43" s="0">
         <v>0</v>
@@ -2402,16 +2402,16 @@
         <v>0</v>
       </c>
       <c r="L43" s="0">
-        <v>20</v>
+        <v>32.666666666666664</v>
       </c>
       <c r="M43" s="0">
-        <v>4.7258156262526088</v>
+        <v>8.3732377913869804</v>
       </c>
       <c r="N43" s="0">
-        <v>116.75321428571418</v>
+        <v>152.85188888888891</v>
       </c>
       <c r="O43" s="0">
-        <v>64.668374692206612</v>
+        <v>59.54986197214258</v>
       </c>
       <c r="P43" s="0">
         <v>0</v>
@@ -2431,22 +2431,22 @@
         <v>7</v>
       </c>
       <c r="D44" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E44" s="0">
         <v>3</v>
       </c>
       <c r="F44" s="0">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G44" s="0">
-        <v>2.5166114784235836</v>
+        <v>4</v>
       </c>
       <c r="H44" s="0">
-        <v>4.666666666666667</v>
+        <v>9.6666666666666661</v>
       </c>
       <c r="I44" s="0">
-        <v>1.3333333333333333</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="J44" s="0">
         <v>0</v>
@@ -2455,16 +2455,16 @@
         <v>0</v>
       </c>
       <c r="L44" s="0">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="M44" s="0">
-        <v>1.7320508075688774</v>
+        <v>4.7258156262526088</v>
       </c>
       <c r="N44" s="0">
-        <v>588.82105555555529</v>
+        <v>116.75321428571418</v>
       </c>
       <c r="O44" s="0">
-        <v>127.10930190851408</v>
+        <v>64.668374692206612</v>
       </c>
       <c r="P44" s="0">
         <v>0</v>
@@ -2484,22 +2484,22 @@
         <v>7</v>
       </c>
       <c r="D45" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E45" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F45" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G45" s="0">
-        <v>0</v>
+        <v>2.5166114784235836</v>
       </c>
       <c r="H45" s="0">
-        <v>0</v>
+        <v>4.666666666666667</v>
       </c>
       <c r="I45" s="0">
-        <v>0</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="J45" s="0">
         <v>0</v>
@@ -2508,16 +2508,16 @@
         <v>0</v>
       </c>
       <c r="L45" s="0">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="M45" s="0">
-        <v>0</v>
+        <v>1.7320508075688774</v>
       </c>
       <c r="N45" s="0">
-        <v>238.08000000000021</v>
+        <v>588.82105555555529</v>
       </c>
       <c r="O45" s="0">
-        <v>0</v>
+        <v>127.10930190851408</v>
       </c>
       <c r="P45" s="0">
         <v>0</v>
@@ -2537,22 +2537,22 @@
         <v>7</v>
       </c>
       <c r="D46" s="0">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E46" s="0">
         <v>3</v>
       </c>
       <c r="F46" s="0">
-        <v>26.666666666666668</v>
+        <v>11</v>
       </c>
       <c r="G46" s="0">
-        <v>20.867305634519386</v>
+        <v>2.5166114784235836</v>
       </c>
       <c r="H46" s="0">
-        <v>7.333333333333333</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="I46" s="0">
-        <v>6.3595946761129714</v>
+        <v>4.0960685758148365</v>
       </c>
       <c r="J46" s="0">
         <v>0</v>
@@ -2561,16 +2561,16 @@
         <v>0</v>
       </c>
       <c r="L46" s="0">
-        <v>30.666666666666668</v>
+        <v>21</v>
       </c>
       <c r="M46" s="0">
-        <v>15.666666666666668</v>
+        <v>3.5118845842842461</v>
       </c>
       <c r="N46" s="0">
-        <v>577.15304444444428</v>
+        <v>509.13412121212133</v>
       </c>
       <c r="O46" s="0">
-        <v>253.34838409883503</v>
+        <v>228.17512271515338</v>
       </c>
       <c r="P46" s="0">
         <v>0</v>
@@ -2590,22 +2590,22 @@
         <v>7</v>
       </c>
       <c r="D47" s="0">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E47" s="0">
         <v>3</v>
       </c>
       <c r="F47" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G47" s="0">
-        <v>6.6583281184793934</v>
+        <v>5.1316014394468841</v>
       </c>
       <c r="H47" s="0">
-        <v>5</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="I47" s="0">
-        <v>2.6457513110645907</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="J47" s="0">
         <v>0</v>
@@ -2614,16 +2614,16 @@
         <v>0</v>
       </c>
       <c r="L47" s="0">
-        <v>28.333333333333332</v>
+        <v>21.666666666666668</v>
       </c>
       <c r="M47" s="0">
-        <v>10.333333333333336</v>
+        <v>6.7659277100614794</v>
       </c>
       <c r="N47" s="0">
-        <v>110.74263888888875</v>
+        <v>112.29188888888895</v>
       </c>
       <c r="O47" s="0">
-        <v>40.400076406244594</v>
+        <v>42.981291669375217</v>
       </c>
       <c r="P47" s="0">
         <v>0</v>
@@ -2643,22 +2643,22 @@
         <v>7</v>
       </c>
       <c r="D48" s="0">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E48" s="0">
         <v>3</v>
       </c>
       <c r="F48" s="0">
-        <v>17.666666666666668</v>
+        <v>26.666666666666668</v>
       </c>
       <c r="G48" s="0">
-        <v>4.9103066208854118</v>
+        <v>20.867305634519386</v>
       </c>
       <c r="H48" s="0">
-        <v>12</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="I48" s="0">
-        <v>1.5275252316519468</v>
+        <v>6.3595946761129714</v>
       </c>
       <c r="J48" s="0">
         <v>0</v>
@@ -2667,16 +2667,16 @@
         <v>0</v>
       </c>
       <c r="L48" s="0">
-        <v>39.333333333333336</v>
+        <v>30.666666666666668</v>
       </c>
       <c r="M48" s="0">
-        <v>7.1724782637833382</v>
+        <v>15.666666666666668</v>
       </c>
       <c r="N48" s="0">
-        <v>199.89207875457876</v>
+        <v>577.15304444444428</v>
       </c>
       <c r="O48" s="0">
-        <v>65.066729994790691</v>
+        <v>253.34838409883503</v>
       </c>
       <c r="P48" s="0">
         <v>0</v>
@@ -2696,40 +2696,40 @@
         <v>7</v>
       </c>
       <c r="D49" s="0">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E49" s="0">
         <v>3</v>
       </c>
       <c r="F49" s="0">
-        <v>30.666666666666668</v>
+        <v>13</v>
       </c>
       <c r="G49" s="0">
-        <v>16.756424970075741</v>
+        <v>6.6583281184793934</v>
       </c>
       <c r="H49" s="0">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="I49" s="0">
-        <v>3.0000000000000004</v>
+        <v>2.6457513110645907</v>
       </c>
       <c r="J49" s="0">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="K49" s="0">
-        <v>9.0737717258774673</v>
+        <v>0</v>
       </c>
       <c r="L49" s="0">
-        <v>19.666666666666668</v>
+        <v>28.333333333333332</v>
       </c>
       <c r="M49" s="0">
-        <v>5.3644923131436935</v>
+        <v>10.333333333333336</v>
       </c>
       <c r="N49" s="0">
-        <v>56.463629072681698</v>
+        <v>110.74263888888875</v>
       </c>
       <c r="O49" s="0">
-        <v>29.939334355348439</v>
+        <v>40.400076406244594</v>
       </c>
       <c r="P49" s="0">
         <v>0</v>
@@ -2740,46 +2740,50 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D50" s="0">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="E50" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F50" s="0">
-        <v>19.25</v>
+        <v>17.666666666666668</v>
       </c>
       <c r="G50" s="0">
-        <v>6.2898728127045622</v>
+        <v>4.9103066208854118</v>
       </c>
       <c r="H50" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="I50" s="0">
-        <v>2.6770630673681683</v>
+        <v>1.5275252316519468</v>
       </c>
       <c r="J50" s="0">
-        <v>8.75</v>
+        <v>0</v>
       </c>
       <c r="K50" s="0">
-        <v>3.0923292192132452</v>
+        <v>0</v>
       </c>
       <c r="L50" s="0">
-        <v>69</v>
+        <v>39.333333333333336</v>
       </c>
       <c r="M50" s="0">
-        <v>15.016657417681207</v>
-      </c>
-      <c r="N50" s="0"/>
-      <c r="O50" s="0"/>
+        <v>7.1724782637833382</v>
+      </c>
+      <c r="N50" s="0">
+        <v>199.89207875457876</v>
+      </c>
+      <c r="O50" s="0">
+        <v>65.066729994790691</v>
+      </c>
       <c r="P50" s="0">
         <v>0</v>
       </c>
@@ -2789,55 +2793,55 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D51" s="0">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E51" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F51" s="0">
-        <v>26.5</v>
+        <v>30.666666666666668</v>
       </c>
       <c r="G51" s="0">
-        <v>14.642973286415115</v>
+        <v>16.756424970075741</v>
       </c>
       <c r="H51" s="0">
-        <v>4.75</v>
+        <v>11</v>
       </c>
       <c r="I51" s="0">
-        <v>1.8874586088176875</v>
+        <v>3.0000000000000004</v>
       </c>
       <c r="J51" s="0">
-        <v>14.25</v>
+        <v>22</v>
       </c>
       <c r="K51" s="0">
-        <v>5.1700257897487001</v>
+        <v>9.0737717258774673</v>
       </c>
       <c r="L51" s="0">
-        <v>94</v>
+        <v>19.666666666666668</v>
       </c>
       <c r="M51" s="0">
-        <v>19.131126469708992</v>
+        <v>5.3644923131436935</v>
       </c>
       <c r="N51" s="0">
-        <v>22.168641025641094</v>
+        <v>56.463629072681698</v>
       </c>
       <c r="O51" s="0">
-        <v>10.533023318956069</v>
+        <v>29.939334355348439</v>
       </c>
       <c r="P51" s="0">
-        <v>49.994060601563049</v>
+        <v>0</v>
       </c>
       <c r="Q51" s="0">
-        <v>19.870402113019829</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -2851,46 +2855,42 @@
         <v>6</v>
       </c>
       <c r="D52" s="0">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E52" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F52" s="0">
-        <v>31</v>
+        <v>19.25</v>
       </c>
       <c r="G52" s="0">
-        <v>10.583005244258363</v>
+        <v>6.2898728127045622</v>
       </c>
       <c r="H52" s="0">
-        <v>8.3333333333333339</v>
+        <v>8</v>
       </c>
       <c r="I52" s="0">
-        <v>3.3333333333333335</v>
+        <v>2.6770630673681683</v>
       </c>
       <c r="J52" s="0">
-        <v>15.333333333333334</v>
+        <v>8.75</v>
       </c>
       <c r="K52" s="0">
-        <v>4.0960685758148365</v>
+        <v>3.0923292192132452</v>
       </c>
       <c r="L52" s="0">
-        <v>50.666666666666664</v>
+        <v>69</v>
       </c>
       <c r="M52" s="0">
-        <v>6.6916199666282443</v>
-      </c>
-      <c r="N52" s="0">
-        <v>33.977886002886017</v>
-      </c>
-      <c r="O52" s="0">
-        <v>13.172894507551444</v>
-      </c>
+        <v>15.016657417681207</v>
+      </c>
+      <c r="N52" s="0"/>
+      <c r="O52" s="0"/>
       <c r="P52" s="0">
-        <v>53.720718787482781</v>
+        <v>0</v>
       </c>
       <c r="Q52" s="0">
-        <v>16.626710579297754</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -2904,46 +2904,46 @@
         <v>6</v>
       </c>
       <c r="D53" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E53" s="0">
         <v>4</v>
       </c>
       <c r="F53" s="0">
-        <v>52</v>
+        <v>26.5</v>
       </c>
       <c r="G53" s="0">
-        <v>13.90443574307614</v>
+        <v>14.642973286415115</v>
       </c>
       <c r="H53" s="0">
-        <v>28</v>
+        <v>4.75</v>
       </c>
       <c r="I53" s="0">
-        <v>16.140012391568973</v>
+        <v>1.8874586088176875</v>
       </c>
       <c r="J53" s="0">
-        <v>32.75</v>
+        <v>14.25</v>
       </c>
       <c r="K53" s="0">
-        <v>7.7714756213561742</v>
+        <v>5.1700257897487001</v>
       </c>
       <c r="L53" s="0">
-        <v>85.25</v>
+        <v>94</v>
       </c>
       <c r="M53" s="0">
-        <v>17.899604278679831</v>
+        <v>19.131126469708992</v>
       </c>
       <c r="N53" s="0">
-        <v>65.366862207602395</v>
+        <v>22.168641025641094</v>
       </c>
       <c r="O53" s="0">
-        <v>32.454443000967174</v>
+        <v>10.533023318956069</v>
       </c>
       <c r="P53" s="0">
-        <v>112.19959175674629</v>
+        <v>49.994060601563049</v>
       </c>
       <c r="Q53" s="0">
-        <v>27.388405886137765</v>
+        <v>19.870402113019829</v>
       </c>
     </row>
     <row r="54">
@@ -2957,46 +2957,46 @@
         <v>6</v>
       </c>
       <c r="D54" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E54" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F54" s="0">
-        <v>42.75</v>
+        <v>31</v>
       </c>
       <c r="G54" s="0">
-        <v>9.0496316683792895</v>
+        <v>10.583005244258363</v>
       </c>
       <c r="H54" s="0">
-        <v>14</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="I54" s="0">
-        <v>3.7638632635454048</v>
+        <v>3.3333333333333335</v>
       </c>
       <c r="J54" s="0">
-        <v>28.25</v>
+        <v>15.333333333333334</v>
       </c>
       <c r="K54" s="0">
-        <v>9.0127224891631208</v>
+        <v>4.0960685758148365</v>
       </c>
       <c r="L54" s="0">
-        <v>46.25</v>
+        <v>50.666666666666664</v>
       </c>
       <c r="M54" s="0">
-        <v>8.6156350123868801</v>
+        <v>6.6916199666282443</v>
       </c>
       <c r="N54" s="0">
-        <v>103.38541508838385</v>
+        <v>33.977886002886017</v>
       </c>
       <c r="O54" s="0">
-        <v>53.774902697870658</v>
+        <v>13.172894507551444</v>
       </c>
       <c r="P54" s="0">
-        <v>94.238180650650094</v>
+        <v>53.720718787482781</v>
       </c>
       <c r="Q54" s="0">
-        <v>27.768089178816695</v>
+        <v>16.626710579297754</v>
       </c>
     </row>
     <row r="55">
@@ -3010,46 +3010,46 @@
         <v>6</v>
       </c>
       <c r="D55" s="0">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E55" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F55" s="0">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="G55" s="0">
-        <v>6.9999999999999991</v>
+        <v>13.90443574307614</v>
       </c>
       <c r="H55" s="0">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="I55" s="0">
-        <v>2</v>
+        <v>16.140012391568973</v>
       </c>
       <c r="J55" s="0">
-        <v>15</v>
+        <v>32.75</v>
       </c>
       <c r="K55" s="0">
-        <v>5</v>
+        <v>7.7714756213561742</v>
       </c>
       <c r="L55" s="0">
-        <v>56.5</v>
+        <v>85.25</v>
       </c>
       <c r="M55" s="0">
-        <v>12.5</v>
+        <v>17.899604278679831</v>
       </c>
       <c r="N55" s="0">
-        <v>56.548749999999984</v>
+        <v>65.366862207602395</v>
       </c>
       <c r="O55" s="0">
-        <v>49.615250000000039</v>
+        <v>32.454443000967174</v>
       </c>
       <c r="P55" s="0">
-        <v>47.681277951699471</v>
+        <v>112.19959175674629</v>
       </c>
       <c r="Q55" s="0">
-        <v>15.188489490161004</v>
+        <v>27.388405886137765</v>
       </c>
     </row>
     <row r="56">
@@ -3063,46 +3063,46 @@
         <v>6</v>
       </c>
       <c r="D56" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E56" s="0">
         <v>4</v>
       </c>
       <c r="F56" s="0">
-        <v>24.5</v>
+        <v>42.75</v>
       </c>
       <c r="G56" s="0">
-        <v>4.7346242371139304</v>
+        <v>9.0496316683792895</v>
       </c>
       <c r="H56" s="0">
-        <v>9.25</v>
+        <v>14</v>
       </c>
       <c r="I56" s="0">
-        <v>1.7017148213885114</v>
+        <v>3.7638632635454048</v>
       </c>
       <c r="J56" s="0">
-        <v>20.25</v>
+        <v>28.25</v>
       </c>
       <c r="K56" s="0">
-        <v>3.2242570203588508</v>
+        <v>9.0127224891631208</v>
       </c>
       <c r="L56" s="0">
-        <v>43.75</v>
+        <v>46.25</v>
       </c>
       <c r="M56" s="0">
-        <v>11.685995892520243</v>
+        <v>8.6156350123868801</v>
       </c>
       <c r="N56" s="0">
-        <v>58.356144480519482</v>
+        <v>103.38541508838385</v>
       </c>
       <c r="O56" s="0">
-        <v>39.025444277436456</v>
+        <v>53.774902697870658</v>
       </c>
       <c r="P56" s="0">
-        <v>66.345643537008328</v>
+        <v>94.238180650650094</v>
       </c>
       <c r="Q56" s="0">
-        <v>10.408746001378843</v>
+        <v>27.768089178816695</v>
       </c>
     </row>
     <row r="57">
@@ -3116,46 +3116,46 @@
         <v>6</v>
       </c>
       <c r="D57" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E57" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F57" s="0">
-        <v>24.75</v>
+        <v>18</v>
       </c>
       <c r="G57" s="0">
-        <v>5.5883062430996624</v>
+        <v>6.9999999999999991</v>
       </c>
       <c r="H57" s="0">
+        <v>4</v>
+      </c>
+      <c r="I57" s="0">
+        <v>2</v>
+      </c>
+      <c r="J57" s="0">
+        <v>15</v>
+      </c>
+      <c r="K57" s="0">
+        <v>5</v>
+      </c>
+      <c r="L57" s="0">
+        <v>56.5</v>
+      </c>
+      <c r="M57" s="0">
         <v>12.5</v>
       </c>
-      <c r="I57" s="0">
-        <v>1.8929694486000912</v>
-      </c>
-      <c r="J57" s="0">
-        <v>19.5</v>
-      </c>
-      <c r="K57" s="0">
-        <v>4.2914643965279113</v>
-      </c>
-      <c r="L57" s="0">
-        <v>42.5</v>
-      </c>
-      <c r="M57" s="0">
-        <v>5.634713834792322</v>
-      </c>
       <c r="N57" s="0">
-        <v>98.323651789386957</v>
+        <v>56.548749999999984</v>
       </c>
       <c r="O57" s="0">
-        <v>43.959531955662413</v>
+        <v>49.615250000000039</v>
       </c>
       <c r="P57" s="0">
-        <v>64.777571457735448</v>
+        <v>47.681277951699471</v>
       </c>
       <c r="Q57" s="0">
-        <v>15.103410376999443</v>
+        <v>15.188489490161004</v>
       </c>
     </row>
     <row r="58">
@@ -3169,46 +3169,46 @@
         <v>6</v>
       </c>
       <c r="D58" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E58" s="0">
         <v>4</v>
       </c>
       <c r="F58" s="0">
-        <v>22.75</v>
+        <v>24.5</v>
       </c>
       <c r="G58" s="0">
-        <v>3.6827299656640586</v>
+        <v>4.7346242371139304</v>
       </c>
       <c r="H58" s="0">
-        <v>8.75</v>
+        <v>9.25</v>
       </c>
       <c r="I58" s="0">
-        <v>2.6887109674836132</v>
+        <v>1.7017148213885114</v>
       </c>
       <c r="J58" s="0">
-        <v>15.25</v>
+        <v>20.25</v>
       </c>
       <c r="K58" s="0">
-        <v>2.2126530078919591</v>
+        <v>3.2242570203588508</v>
       </c>
       <c r="L58" s="0">
-        <v>47</v>
+        <v>43.75</v>
       </c>
       <c r="M58" s="0">
-        <v>12.935738607954837</v>
+        <v>11.685995892520243</v>
       </c>
       <c r="N58" s="0">
-        <v>157.92080176767675</v>
+        <v>58.356144480519482</v>
       </c>
       <c r="O58" s="0">
-        <v>83.227737171056702</v>
+        <v>39.025444277436456</v>
       </c>
       <c r="P58" s="0">
-        <v>50.256551304898892</v>
+        <v>66.345643537008328</v>
       </c>
       <c r="Q58" s="0">
-        <v>7.7511695070748141</v>
+        <v>10.408746001378843</v>
       </c>
     </row>
     <row r="59">
@@ -3222,46 +3222,46 @@
         <v>6</v>
       </c>
       <c r="D59" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E59" s="0">
         <v>4</v>
       </c>
       <c r="F59" s="0">
-        <v>29.5</v>
+        <v>24.75</v>
       </c>
       <c r="G59" s="0">
-        <v>4.1733280085163047</v>
+        <v>5.5883062430996624</v>
       </c>
       <c r="H59" s="0">
-        <v>5.75</v>
+        <v>12.5</v>
       </c>
       <c r="I59" s="0">
-        <v>1.4930394055974097</v>
+        <v>1.8929694486000912</v>
       </c>
       <c r="J59" s="0">
-        <v>19.75</v>
+        <v>19.5</v>
       </c>
       <c r="K59" s="0">
-        <v>2.2867371223353739</v>
+        <v>4.2914643965279113</v>
       </c>
       <c r="L59" s="0">
-        <v>50.75</v>
+        <v>42.5</v>
       </c>
       <c r="M59" s="0">
-        <v>16.131620088096131</v>
+        <v>5.634713834792322</v>
       </c>
       <c r="N59" s="0">
-        <v>65.46980357142867</v>
+        <v>98.323651789386957</v>
       </c>
       <c r="O59" s="0">
-        <v>42.191087062516566</v>
+        <v>43.959531955662413</v>
       </c>
       <c r="P59" s="0">
-        <v>64.147899335807864</v>
+        <v>64.777571457735448</v>
       </c>
       <c r="Q59" s="0">
-        <v>5.9704849097917378</v>
+        <v>15.103410376999443</v>
       </c>
     </row>
     <row r="60">
@@ -3275,46 +3275,46 @@
         <v>6</v>
       </c>
       <c r="D60" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E60" s="0">
         <v>4</v>
       </c>
       <c r="F60" s="0">
-        <v>26.25</v>
+        <v>22.75</v>
       </c>
       <c r="G60" s="0">
-        <v>6.3688696014284982</v>
+        <v>3.6827299656640586</v>
       </c>
       <c r="H60" s="0">
-        <v>5</v>
+        <v>8.75</v>
       </c>
       <c r="I60" s="0">
-        <v>1.2909944487358056</v>
+        <v>2.6887109674836132</v>
       </c>
       <c r="J60" s="0">
-        <v>19.5</v>
+        <v>15.25</v>
       </c>
       <c r="K60" s="0">
-        <v>4.4253060157839181</v>
+        <v>2.2126530078919591</v>
       </c>
       <c r="L60" s="0">
-        <v>52.25</v>
+        <v>47</v>
       </c>
       <c r="M60" s="0">
-        <v>7.3979163733220625</v>
+        <v>12.935738607954837</v>
       </c>
       <c r="N60" s="0">
-        <v>76.725373376623381</v>
+        <v>157.92080176767675</v>
       </c>
       <c r="O60" s="0">
-        <v>69.106430857045268</v>
+        <v>83.227737171056702</v>
       </c>
       <c r="P60" s="0">
-        <v>63.31241883365562</v>
+        <v>50.256551304898892</v>
       </c>
       <c r="Q60" s="0">
-        <v>13.870452293565409</v>
+        <v>7.7511695070748141</v>
       </c>
     </row>
     <row r="61">
@@ -3328,46 +3328,46 @@
         <v>6</v>
       </c>
       <c r="D61" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E61" s="0">
         <v>4</v>
       </c>
       <c r="F61" s="0">
-        <v>25.75</v>
+        <v>29.5</v>
       </c>
       <c r="G61" s="0">
-        <v>3.966001344763598</v>
+        <v>4.1733280085163047</v>
       </c>
       <c r="H61" s="0">
-        <v>4.5</v>
+        <v>5.75</v>
       </c>
       <c r="I61" s="0">
-        <v>1.9364916731037085</v>
+        <v>1.4930394055974097</v>
       </c>
       <c r="J61" s="0">
-        <v>20.25</v>
+        <v>19.75</v>
       </c>
       <c r="K61" s="0">
-        <v>2.0155644370746373</v>
+        <v>2.2867371223353739</v>
       </c>
       <c r="L61" s="0">
-        <v>48.25</v>
+        <v>50.75</v>
       </c>
       <c r="M61" s="0">
-        <v>11.360567767501763</v>
+        <v>16.131620088096131</v>
       </c>
       <c r="N61" s="0">
-        <v>51.138666666666744</v>
+        <v>65.46980357142867</v>
       </c>
       <c r="O61" s="0">
-        <v>40.114655891304643</v>
+        <v>42.191087062516566</v>
       </c>
       <c r="P61" s="0">
-        <v>64.238335695371177</v>
+        <v>64.147899335807864</v>
       </c>
       <c r="Q61" s="0">
-        <v>4.4645526493660395</v>
+        <v>5.9704849097917378</v>
       </c>
     </row>
     <row r="62">
@@ -3381,46 +3381,46 @@
         <v>6</v>
       </c>
       <c r="D62" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E62" s="0">
         <v>4</v>
       </c>
       <c r="F62" s="0">
-        <v>42.75</v>
+        <v>26.25</v>
       </c>
       <c r="G62" s="0">
-        <v>10.019772119830536</v>
+        <v>6.3688696014284982</v>
       </c>
       <c r="H62" s="0">
         <v>5</v>
       </c>
       <c r="I62" s="0">
-        <v>1.6329931618554521</v>
+        <v>1.2909944487358056</v>
       </c>
       <c r="J62" s="0">
-        <v>28.75</v>
+        <v>19.5</v>
       </c>
       <c r="K62" s="0">
-        <v>5.7789128158619363</v>
+        <v>4.4253060157839181</v>
       </c>
       <c r="L62" s="0">
-        <v>44.75</v>
+        <v>52.25</v>
       </c>
       <c r="M62" s="0">
-        <v>5.7644745351737541</v>
+        <v>7.3979163733220625</v>
       </c>
       <c r="N62" s="0">
-        <v>25.704719336219309</v>
+        <v>76.725373376623381</v>
       </c>
       <c r="O62" s="0">
-        <v>15.641396975578967</v>
+        <v>69.106430857045268</v>
       </c>
       <c r="P62" s="0">
-        <v>94.175646488409257</v>
+        <v>63.31241883365562</v>
       </c>
       <c r="Q62" s="0">
-        <v>23.051089999527441</v>
+        <v>13.870452293565409</v>
       </c>
     </row>
     <row r="63">
@@ -3434,46 +3434,46 @@
         <v>6</v>
       </c>
       <c r="D63" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E63" s="0">
         <v>4</v>
       </c>
       <c r="F63" s="0">
-        <v>32.75</v>
+        <v>25.75</v>
       </c>
       <c r="G63" s="0">
-        <v>3.0652623596249202</v>
+        <v>3.966001344763598</v>
       </c>
       <c r="H63" s="0">
-        <v>10.75</v>
+        <v>4.5</v>
       </c>
       <c r="I63" s="0">
-        <v>3.727711541057507</v>
+        <v>1.9364916731037085</v>
       </c>
       <c r="J63" s="0">
-        <v>24.75</v>
+        <v>20.25</v>
       </c>
       <c r="K63" s="0">
-        <v>1.796988221070652</v>
+        <v>2.0155644370746373</v>
       </c>
       <c r="L63" s="0">
-        <v>56.25</v>
+        <v>48.25</v>
       </c>
       <c r="M63" s="0">
-        <v>15.195256935416833</v>
+        <v>11.360567767501763</v>
       </c>
       <c r="N63" s="0">
-        <v>28.258526785714359</v>
+        <v>51.138666666666744</v>
       </c>
       <c r="O63" s="0">
-        <v>9.0461220240131937</v>
+        <v>40.114655891304643</v>
       </c>
       <c r="P63" s="0">
-        <v>79.812837679384813</v>
+        <v>64.238335695371177</v>
       </c>
       <c r="Q63" s="0">
-        <v>8.992374134090074</v>
+        <v>4.4645526493660395</v>
       </c>
     </row>
     <row r="64">
@@ -3487,46 +3487,46 @@
         <v>6</v>
       </c>
       <c r="D64" s="0">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E64" s="0">
         <v>4</v>
       </c>
       <c r="F64" s="0">
-        <v>37</v>
+        <v>42.75</v>
       </c>
       <c r="G64" s="0">
-        <v>1.9578900207451218</v>
+        <v>10.019772119830536</v>
       </c>
       <c r="H64" s="0">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="I64" s="0">
-        <v>1.2583057392117916</v>
+        <v>1.6329931618554521</v>
       </c>
       <c r="J64" s="0">
-        <v>23.25</v>
+        <v>28.75</v>
       </c>
       <c r="K64" s="0">
-        <v>2.3228933107943921</v>
+        <v>5.7789128158619363</v>
       </c>
       <c r="L64" s="0">
-        <v>40.25</v>
+        <v>44.75</v>
       </c>
       <c r="M64" s="0">
-        <v>11.145813862911343</v>
+        <v>5.7644745351737541</v>
       </c>
       <c r="N64" s="0">
-        <v>47.795265700483078</v>
+        <v>25.704719336219309</v>
       </c>
       <c r="O64" s="0">
-        <v>27.238849941220227</v>
+        <v>15.641396975578967</v>
       </c>
       <c r="P64" s="0">
-        <v>73.660580051462745</v>
+        <v>94.175646488409257</v>
       </c>
       <c r="Q64" s="0">
-        <v>5.450846864686576</v>
+        <v>23.051089999527441</v>
       </c>
     </row>
     <row r="65">
@@ -3540,46 +3540,46 @@
         <v>6</v>
       </c>
       <c r="D65" s="0">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E65" s="0">
         <v>4</v>
       </c>
       <c r="F65" s="0">
-        <v>27.5</v>
+        <v>32.75</v>
       </c>
       <c r="G65" s="0">
-        <v>3.7969285832981723</v>
+        <v>3.0652623596249202</v>
       </c>
       <c r="H65" s="0">
-        <v>4.75</v>
+        <v>10.75</v>
       </c>
       <c r="I65" s="0">
-        <v>1.25</v>
+        <v>3.727711541057507</v>
       </c>
       <c r="J65" s="0">
-        <v>18.75</v>
+        <v>24.75</v>
       </c>
       <c r="K65" s="0">
-        <v>3.6371921404658658</v>
+        <v>1.796988221070652</v>
       </c>
       <c r="L65" s="0">
-        <v>44.25</v>
+        <v>56.25</v>
       </c>
       <c r="M65" s="0">
-        <v>11.778334630441888</v>
+        <v>15.195256935416833</v>
       </c>
       <c r="N65" s="0">
-        <v>88.2486706349207</v>
+        <v>28.258526785714359</v>
       </c>
       <c r="O65" s="0">
-        <v>51.947599644891973</v>
+        <v>9.0461220240131937</v>
       </c>
       <c r="P65" s="0">
-        <v>58.745823293261395</v>
+        <v>79.812837679384813</v>
       </c>
       <c r="Q65" s="0">
-        <v>9.2946014595546824</v>
+        <v>8.992374134090074</v>
       </c>
     </row>
     <row r="66">
@@ -3593,46 +3593,46 @@
         <v>6</v>
       </c>
       <c r="D66" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E66" s="0">
         <v>4</v>
       </c>
       <c r="F66" s="0">
-        <v>62.5</v>
+        <v>37</v>
       </c>
       <c r="G66" s="0">
-        <v>14.038637160826308</v>
+        <v>1.9578900207451218</v>
       </c>
       <c r="H66" s="0">
-        <v>33.25</v>
+        <v>6.5</v>
       </c>
       <c r="I66" s="0">
-        <v>6.884463184107628</v>
+        <v>1.2583057392117916</v>
       </c>
       <c r="J66" s="0">
-        <v>0</v>
+        <v>23.25</v>
       </c>
       <c r="K66" s="0">
-        <v>0</v>
+        <v>2.3228933107943921</v>
       </c>
       <c r="L66" s="0">
-        <v>71.25</v>
+        <v>40.25</v>
       </c>
       <c r="M66" s="0">
-        <v>20.25</v>
+        <v>11.145813862911343</v>
       </c>
       <c r="N66" s="0">
-        <v>141.62886195690896</v>
+        <v>47.795265700483078</v>
       </c>
       <c r="O66" s="0">
-        <v>82.359639827192964</v>
+        <v>27.238849941220227</v>
       </c>
       <c r="P66" s="0">
-        <v>0</v>
+        <v>73.660580051462745</v>
       </c>
       <c r="Q66" s="0">
-        <v>0</v>
+        <v>5.450846864686576</v>
       </c>
     </row>
     <row r="67">
@@ -3646,46 +3646,46 @@
         <v>6</v>
       </c>
       <c r="D67" s="0">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E67" s="0">
         <v>4</v>
       </c>
       <c r="F67" s="0">
-        <v>36</v>
+        <v>27.5</v>
       </c>
       <c r="G67" s="0">
-        <v>13.435028842544403</v>
+        <v>3.7969285832981723</v>
       </c>
       <c r="H67" s="0">
-        <v>30.5</v>
+        <v>4.75</v>
       </c>
       <c r="I67" s="0">
-        <v>7.5993420767853319</v>
+        <v>1.25</v>
       </c>
       <c r="J67" s="0">
-        <v>0</v>
+        <v>18.75</v>
       </c>
       <c r="K67" s="0">
-        <v>0</v>
+        <v>3.6371921404658658</v>
       </c>
       <c r="L67" s="0">
-        <v>56</v>
+        <v>44.25</v>
       </c>
       <c r="M67" s="0">
-        <v>18.677080428518085</v>
+        <v>11.778334630441888</v>
       </c>
       <c r="N67" s="0">
-        <v>107.25609910714282</v>
+        <v>88.2486706349207</v>
       </c>
       <c r="O67" s="0">
-        <v>29.781670816218028</v>
+        <v>51.947599644891973</v>
       </c>
       <c r="P67" s="0">
-        <v>0</v>
+        <v>58.745823293261395</v>
       </c>
       <c r="Q67" s="0">
-        <v>0</v>
+        <v>9.2946014595546824</v>
       </c>
     </row>
     <row r="68">
@@ -3699,22 +3699,22 @@
         <v>6</v>
       </c>
       <c r="D68" s="0">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E68" s="0">
         <v>4</v>
       </c>
       <c r="F68" s="0">
-        <v>37.75</v>
+        <v>62.5</v>
       </c>
       <c r="G68" s="0">
-        <v>14.4185933202006</v>
+        <v>14.038637160826308</v>
       </c>
       <c r="H68" s="0">
-        <v>29.25</v>
+        <v>33.25</v>
       </c>
       <c r="I68" s="0">
-        <v>8.4594621578443157</v>
+        <v>6.884463184107628</v>
       </c>
       <c r="J68" s="0">
         <v>0</v>
@@ -3723,16 +3723,16 @@
         <v>0</v>
       </c>
       <c r="L68" s="0">
-        <v>39.75</v>
+        <v>71.25</v>
       </c>
       <c r="M68" s="0">
-        <v>6.9447222166668885</v>
+        <v>20.25</v>
       </c>
       <c r="N68" s="0">
-        <v>181.41195138888884</v>
+        <v>141.62886195690896</v>
       </c>
       <c r="O68" s="0">
-        <v>33.385075537981827</v>
+        <v>82.359639827192964</v>
       </c>
       <c r="P68" s="0">
         <v>0</v>
@@ -3752,22 +3752,22 @@
         <v>6</v>
       </c>
       <c r="D69" s="0">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E69" s="0">
         <v>4</v>
       </c>
       <c r="F69" s="0">
-        <v>24.75</v>
+        <v>36</v>
       </c>
       <c r="G69" s="0">
-        <v>7.4763516057856281</v>
+        <v>13.435028842544403</v>
       </c>
       <c r="H69" s="0">
-        <v>22.5</v>
+        <v>30.5</v>
       </c>
       <c r="I69" s="0">
-        <v>7.4665922615340392</v>
+        <v>7.5993420767853319</v>
       </c>
       <c r="J69" s="0">
         <v>0</v>
@@ -3776,16 +3776,16 @@
         <v>0</v>
       </c>
       <c r="L69" s="0">
-        <v>45.75</v>
+        <v>56</v>
       </c>
       <c r="M69" s="0">
-        <v>18.454335533960577</v>
+        <v>18.677080428518085</v>
       </c>
       <c r="N69" s="0">
-        <v>99.65195833333334</v>
+        <v>107.25609910714282</v>
       </c>
       <c r="O69" s="0">
-        <v>21.13483940549774</v>
+        <v>29.781670816218028</v>
       </c>
       <c r="P69" s="0">
         <v>0</v>
@@ -3805,22 +3805,22 @@
         <v>6</v>
       </c>
       <c r="D70" s="0">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E70" s="0">
         <v>4</v>
       </c>
       <c r="F70" s="0">
-        <v>26.5</v>
+        <v>37.75</v>
       </c>
       <c r="G70" s="0">
-        <v>7.0296989029877137</v>
+        <v>14.4185933202006</v>
       </c>
       <c r="H70" s="0">
-        <v>17</v>
+        <v>29.25</v>
       </c>
       <c r="I70" s="0">
-        <v>7.32575365861197</v>
+        <v>8.4594621578443157</v>
       </c>
       <c r="J70" s="0">
         <v>0</v>
@@ -3829,16 +3829,16 @@
         <v>0</v>
       </c>
       <c r="L70" s="0">
-        <v>42</v>
+        <v>39.75</v>
       </c>
       <c r="M70" s="0">
-        <v>14.462595433277757</v>
+        <v>6.9447222166668885</v>
       </c>
       <c r="N70" s="0">
-        <v>90.338575320512774</v>
+        <v>181.41195138888884</v>
       </c>
       <c r="O70" s="0">
-        <v>22.621184296690576</v>
+        <v>33.385075537981827</v>
       </c>
       <c r="P70" s="0">
         <v>0</v>
@@ -3858,22 +3858,22 @@
         <v>6</v>
       </c>
       <c r="D71" s="0">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E71" s="0">
         <v>4</v>
       </c>
       <c r="F71" s="0">
-        <v>15.75</v>
+        <v>22.75</v>
       </c>
       <c r="G71" s="0">
-        <v>4.8196645803070846</v>
+        <v>6.0466933112239118</v>
       </c>
       <c r="H71" s="0">
-        <v>22.25</v>
+        <v>20</v>
       </c>
       <c r="I71" s="0">
-        <v>6.459811658761164</v>
+        <v>6.1373175465073224</v>
       </c>
       <c r="J71" s="0">
         <v>0</v>
@@ -3882,16 +3882,16 @@
         <v>0</v>
       </c>
       <c r="L71" s="0">
-        <v>24.5</v>
+        <v>52.5</v>
       </c>
       <c r="M71" s="0">
-        <v>6.1846584384264904</v>
+        <v>14.262421486783605</v>
       </c>
       <c r="N71" s="0">
-        <v>731.94416666666677</v>
+        <v>454.76208333333329</v>
       </c>
       <c r="O71" s="0">
-        <v>353.11125512676108</v>
+        <v>262.27775600688477</v>
       </c>
       <c r="P71" s="0">
         <v>0</v>
@@ -3911,40 +3911,40 @@
         <v>6</v>
       </c>
       <c r="D72" s="0">
+        <v>20</v>
+      </c>
+      <c r="E72" s="0">
+        <v>4</v>
+      </c>
+      <c r="F72" s="0">
+        <v>17</v>
+      </c>
+      <c r="G72" s="0">
+        <v>5.873670062235365</v>
+      </c>
+      <c r="H72" s="0">
         <v>24</v>
       </c>
-      <c r="E72" s="0">
-        <v>4</v>
-      </c>
-      <c r="F72" s="0">
-        <v>21</v>
-      </c>
-      <c r="G72" s="0">
-        <v>8.9721792224631809</v>
-      </c>
-      <c r="H72" s="0">
-        <v>15.25</v>
-      </c>
       <c r="I72" s="0">
-        <v>3.6371921404658658</v>
+        <v>8.7844559687362924</v>
       </c>
       <c r="J72" s="0">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="K72" s="0">
-        <v>4.9665548085837798</v>
+        <v>0</v>
       </c>
       <c r="L72" s="0">
-        <v>28.75</v>
+        <v>37</v>
       </c>
       <c r="M72" s="0">
-        <v>9.32179346120334</v>
+        <v>16.299284237863535</v>
       </c>
       <c r="N72" s="0">
-        <v>24.689971988795534</v>
+        <v>296.84473484848496</v>
       </c>
       <c r="O72" s="0">
-        <v>12.357842110394305</v>
+        <v>219.87051855522139</v>
       </c>
       <c r="P72" s="0">
         <v>0</v>
@@ -3961,40 +3961,44 @@
         <v>4</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D73" s="0">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E73" s="0">
         <v>4</v>
       </c>
       <c r="F73" s="0">
-        <v>11.5</v>
+        <v>24.75</v>
       </c>
       <c r="G73" s="0">
-        <v>3.378855822118882</v>
+        <v>7.4763516057856281</v>
       </c>
       <c r="H73" s="0">
-        <v>5.75</v>
+        <v>22.5</v>
       </c>
       <c r="I73" s="0">
-        <v>1.1086778913041726</v>
+        <v>7.4665922615340392</v>
       </c>
       <c r="J73" s="0">
-        <v>6.75</v>
+        <v>0</v>
       </c>
       <c r="K73" s="0">
-        <v>1.973786547054502</v>
+        <v>0</v>
       </c>
       <c r="L73" s="0">
-        <v>26.75</v>
+        <v>45.75</v>
       </c>
       <c r="M73" s="0">
-        <v>2.5289984842489197</v>
-      </c>
-      <c r="N73" s="0"/>
-      <c r="O73" s="0"/>
+        <v>18.454335533960577</v>
+      </c>
+      <c r="N73" s="0">
+        <v>99.65195833333334</v>
+      </c>
+      <c r="O73" s="0">
+        <v>21.13483940549774</v>
+      </c>
       <c r="P73" s="0">
         <v>0</v>
       </c>
@@ -4010,49 +4014,49 @@
         <v>4</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D74" s="0">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="E74" s="0">
         <v>4</v>
       </c>
       <c r="F74" s="0">
-        <v>29.75</v>
+        <v>26.5</v>
       </c>
       <c r="G74" s="0">
-        <v>12.51915199471061</v>
+        <v>7.0296989029877137</v>
       </c>
       <c r="H74" s="0">
-        <v>5.5</v>
+        <v>17</v>
       </c>
       <c r="I74" s="0">
-        <v>2.5331140255951108</v>
+        <v>7.32575365861197</v>
       </c>
       <c r="J74" s="0">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="K74" s="0">
-        <v>6.324555320336759</v>
+        <v>0</v>
       </c>
       <c r="L74" s="0">
-        <v>49.75</v>
+        <v>42</v>
       </c>
       <c r="M74" s="0">
-        <v>11.678862672937521</v>
+        <v>14.462595433277757</v>
       </c>
       <c r="N74" s="0">
-        <v>199.02467307692302</v>
+        <v>90.338575320512774</v>
       </c>
       <c r="O74" s="0">
-        <v>83.158139318497049</v>
+        <v>22.621184296690576</v>
       </c>
       <c r="P74" s="0">
-        <v>56.220744202549618</v>
+        <v>0</v>
       </c>
       <c r="Q74" s="0">
-        <v>19.425478785356162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -4063,49 +4067,49 @@
         <v>4</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D75" s="0">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="E75" s="0">
         <v>4</v>
       </c>
       <c r="F75" s="0">
-        <v>28.5</v>
+        <v>15.75</v>
       </c>
       <c r="G75" s="0">
-        <v>8.4606934309980364</v>
+        <v>4.8196645803070846</v>
       </c>
       <c r="H75" s="0">
-        <v>4.5</v>
+        <v>22.25</v>
       </c>
       <c r="I75" s="0">
-        <v>1.0408329997330663</v>
+        <v>6.459811658761164</v>
       </c>
       <c r="J75" s="0">
-        <v>18.25</v>
+        <v>0</v>
       </c>
       <c r="K75" s="0">
-        <v>5.5283360968739954</v>
+        <v>0</v>
       </c>
       <c r="L75" s="0">
-        <v>16.5</v>
+        <v>24.5</v>
       </c>
       <c r="M75" s="0">
-        <v>4.0926763859362252</v>
+        <v>6.1846584384264904</v>
       </c>
       <c r="N75" s="0">
-        <v>123.76519444444445</v>
+        <v>731.94416666666677</v>
       </c>
       <c r="O75" s="0">
-        <v>96.563654110602727</v>
+        <v>353.11125512676108</v>
       </c>
       <c r="P75" s="0">
-        <v>57.096024507691922</v>
+        <v>0</v>
       </c>
       <c r="Q75" s="0">
-        <v>17.581199231611976</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -4116,49 +4120,49 @@
         <v>4</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D76" s="0">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E76" s="0">
         <v>4</v>
       </c>
       <c r="F76" s="0">
-        <v>54.25</v>
+        <v>21</v>
       </c>
       <c r="G76" s="0">
-        <v>23.264332499916403</v>
+        <v>8.9721792224631809</v>
       </c>
       <c r="H76" s="0">
+        <v>15.25</v>
+      </c>
+      <c r="I76" s="0">
+        <v>3.6371921404658658</v>
+      </c>
+      <c r="J76" s="0">
         <v>12</v>
       </c>
-      <c r="I76" s="0">
-        <v>5.8166427888717163</v>
-      </c>
-      <c r="J76" s="0">
-        <v>37</v>
-      </c>
       <c r="K76" s="0">
-        <v>16.416455159382004</v>
+        <v>4.9665548085837798</v>
       </c>
       <c r="L76" s="0">
-        <v>29.25</v>
+        <v>28.75</v>
       </c>
       <c r="M76" s="0">
-        <v>7.1922991224410753</v>
+        <v>9.32179346120334</v>
       </c>
       <c r="N76" s="0">
-        <v>396.74887121212117</v>
+        <v>24.689971988795534</v>
       </c>
       <c r="O76" s="0">
-        <v>320.97552634128039</v>
+        <v>12.357842110394305</v>
       </c>
       <c r="P76" s="0">
-        <v>114.90023813898675</v>
+        <v>0</v>
       </c>
       <c r="Q76" s="0">
-        <v>50.044468626942816</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -4172,46 +4176,42 @@
         <v>7</v>
       </c>
       <c r="D77" s="0">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E77" s="0">
         <v>4</v>
       </c>
       <c r="F77" s="0">
-        <v>37.25</v>
+        <v>11.5</v>
       </c>
       <c r="G77" s="0">
-        <v>15.939338129295081</v>
+        <v>3.378855822118882</v>
       </c>
       <c r="H77" s="0">
         <v>5.75</v>
       </c>
       <c r="I77" s="0">
-        <v>2.462214450449026</v>
+        <v>1.1086778913041726</v>
       </c>
       <c r="J77" s="0">
-        <v>30.5</v>
+        <v>6.75</v>
       </c>
       <c r="K77" s="0">
-        <v>12.038133853162901</v>
+        <v>1.973786547054502</v>
       </c>
       <c r="L77" s="0">
-        <v>24.25</v>
+        <v>26.75</v>
       </c>
       <c r="M77" s="0">
-        <v>8.3404136588061384</v>
-      </c>
-      <c r="N77" s="0">
-        <v>134.40125000000003</v>
-      </c>
-      <c r="O77" s="0">
-        <v>67.057948079527264</v>
-      </c>
+        <v>2.5289984842489197</v>
+      </c>
+      <c r="N77" s="0"/>
+      <c r="O77" s="0"/>
       <c r="P77" s="0">
-        <v>95.023410332767327</v>
+        <v>0</v>
       </c>
       <c r="Q77" s="0">
-        <v>36.817250218707393</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -4225,46 +4225,46 @@
         <v>7</v>
       </c>
       <c r="D78" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E78" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F78" s="0">
-        <v>50.5</v>
+        <v>29.75</v>
       </c>
       <c r="G78" s="0">
-        <v>45.499999999999993</v>
+        <v>12.51915199471061</v>
       </c>
       <c r="H78" s="0">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="I78" s="0">
-        <v>2.9999999999999996</v>
+        <v>2.5331140255951108</v>
       </c>
       <c r="J78" s="0">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="K78" s="0">
-        <v>33.999999999999993</v>
+        <v>6.324555320336759</v>
       </c>
       <c r="L78" s="0">
-        <v>15.5</v>
+        <v>49.75</v>
       </c>
       <c r="M78" s="0">
-        <v>7.5</v>
+        <v>11.678862672937521</v>
       </c>
       <c r="N78" s="0">
-        <v>587.1704545454545</v>
+        <v>199.02467307692302</v>
       </c>
       <c r="O78" s="0">
-        <v>570.04954545454541</v>
+        <v>83.158139318497049</v>
       </c>
       <c r="P78" s="0">
-        <v>120.13736051271005</v>
+        <v>56.220744202549618</v>
       </c>
       <c r="Q78" s="0">
-        <v>104.12195766910814</v>
+        <v>19.425478785356162</v>
       </c>
     </row>
     <row r="79">
@@ -4278,46 +4278,46 @@
         <v>7</v>
       </c>
       <c r="D79" s="0">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E79" s="0">
         <v>4</v>
       </c>
       <c r="F79" s="0">
-        <v>26</v>
+        <v>28.5</v>
       </c>
       <c r="G79" s="0">
-        <v>9.9582461641931044</v>
+        <v>8.4606934309980364</v>
       </c>
       <c r="H79" s="0">
-        <v>6.75</v>
+        <v>4.5</v>
       </c>
       <c r="I79" s="0">
-        <v>2.6575364531836625</v>
+        <v>1.0408329997330663</v>
       </c>
       <c r="J79" s="0">
-        <v>20.75</v>
+        <v>18.25</v>
       </c>
       <c r="K79" s="0">
-        <v>8.1687922403906601</v>
+        <v>5.5283360968739954</v>
       </c>
       <c r="L79" s="0">
-        <v>22.5</v>
+        <v>16.5</v>
       </c>
       <c r="M79" s="0">
-        <v>4.1932485418030412</v>
+        <v>4.0926763859362252</v>
       </c>
       <c r="N79" s="0">
-        <v>347.29934920634918</v>
+        <v>123.76519444444445</v>
       </c>
       <c r="O79" s="0">
-        <v>158.54349546179873</v>
+        <v>96.563654110602727</v>
       </c>
       <c r="P79" s="0">
-        <v>61.087244108135195</v>
+        <v>57.096024507691922</v>
       </c>
       <c r="Q79" s="0">
-        <v>23.644092541978718</v>
+        <v>17.581199231611976</v>
       </c>
     </row>
     <row r="80">
@@ -4331,46 +4331,46 @@
         <v>7</v>
       </c>
       <c r="D80" s="0">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E80" s="0">
         <v>4</v>
       </c>
       <c r="F80" s="0">
-        <v>22.75</v>
+        <v>54.25</v>
       </c>
       <c r="G80" s="0">
-        <v>7.9621500446382782</v>
+        <v>23.264332499916403</v>
       </c>
       <c r="H80" s="0">
-        <v>3.75</v>
+        <v>12</v>
       </c>
       <c r="I80" s="0">
-        <v>1.6520189667999174</v>
+        <v>5.8166427888717163</v>
       </c>
       <c r="J80" s="0">
-        <v>20.25</v>
+        <v>37</v>
       </c>
       <c r="K80" s="0">
-        <v>7.2154348448309058</v>
+        <v>16.416455159382004</v>
       </c>
       <c r="L80" s="0">
-        <v>22.75</v>
+        <v>29.25</v>
       </c>
       <c r="M80" s="0">
-        <v>7.9201746613737418</v>
+        <v>7.1922991224410753</v>
       </c>
       <c r="N80" s="0">
-        <v>708.12724358974367</v>
+        <v>396.74887121212117</v>
       </c>
       <c r="O80" s="0">
-        <v>561.21766446431354</v>
+        <v>320.97552634128039</v>
       </c>
       <c r="P80" s="0">
-        <v>59.918759272660409</v>
+        <v>114.90023813898675</v>
       </c>
       <c r="Q80" s="0">
-        <v>21.035766353192841</v>
+        <v>50.044468626942816</v>
       </c>
     </row>
     <row r="81">
@@ -4384,46 +4384,46 @@
         <v>7</v>
       </c>
       <c r="D81" s="0">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E81" s="0">
         <v>4</v>
       </c>
       <c r="F81" s="0">
-        <v>33.25</v>
+        <v>37.25</v>
       </c>
       <c r="G81" s="0">
-        <v>5.1051444641655346</v>
+        <v>15.939338129295081</v>
       </c>
       <c r="H81" s="0">
-        <v>7.5</v>
+        <v>5.75</v>
       </c>
       <c r="I81" s="0">
-        <v>2.5331140255951108</v>
+        <v>2.462214450449026</v>
       </c>
       <c r="J81" s="0">
-        <v>25.75</v>
+        <v>30.5</v>
       </c>
       <c r="K81" s="0">
-        <v>3.6371921404658658</v>
+        <v>12.038133853162901</v>
       </c>
       <c r="L81" s="0">
         <v>24.25</v>
       </c>
       <c r="M81" s="0">
-        <v>4.7147817199385456</v>
+        <v>8.3404136588061384</v>
       </c>
       <c r="N81" s="0">
-        <v>142.98126893939397</v>
+        <v>134.40125000000003</v>
       </c>
       <c r="O81" s="0">
-        <v>36.959966323550475</v>
+        <v>67.057948079527264</v>
       </c>
       <c r="P81" s="0">
-        <v>75.952174842019758</v>
+        <v>95.023410332767327</v>
       </c>
       <c r="Q81" s="0">
-        <v>10.026028158088602</v>
+        <v>36.817250218707393</v>
       </c>
     </row>
     <row r="82">
@@ -4437,46 +4437,46 @@
         <v>7</v>
       </c>
       <c r="D82" s="0">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E82" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F82" s="0">
-        <v>17.25</v>
+        <v>50.5</v>
       </c>
       <c r="G82" s="0">
-        <v>4.732423621500228</v>
+        <v>45.499999999999993</v>
       </c>
       <c r="H82" s="0">
-        <v>9.25</v>
+        <v>4</v>
       </c>
       <c r="I82" s="0">
-        <v>6.9686799323831767</v>
+        <v>2.9999999999999996</v>
       </c>
       <c r="J82" s="0">
-        <v>14.25</v>
+        <v>39</v>
       </c>
       <c r="K82" s="0">
-        <v>4.4040700872412701</v>
+        <v>33.999999999999993</v>
       </c>
       <c r="L82" s="0">
-        <v>31</v>
+        <v>15.5</v>
       </c>
       <c r="M82" s="0">
-        <v>18.605554726120548</v>
+        <v>7.5</v>
       </c>
       <c r="N82" s="0">
-        <v>306.30527777777775</v>
+        <v>587.1704545454545</v>
       </c>
       <c r="O82" s="0">
-        <v>144.64282161794904</v>
+        <v>570.04954545454541</v>
       </c>
       <c r="P82" s="0">
-        <v>42.255216679264713</v>
+        <v>120.13736051271005</v>
       </c>
       <c r="Q82" s="0">
-        <v>13.15467278835462</v>
+        <v>104.12195766910814</v>
       </c>
     </row>
     <row r="83">
@@ -4490,46 +4490,46 @@
         <v>7</v>
       </c>
       <c r="D83" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E83" s="0">
         <v>4</v>
       </c>
       <c r="F83" s="0">
-        <v>16.25</v>
+        <v>26</v>
       </c>
       <c r="G83" s="0">
-        <v>5.5733742024019888</v>
+        <v>9.9582461641931044</v>
       </c>
       <c r="H83" s="0">
-        <v>1</v>
+        <v>6.75</v>
       </c>
       <c r="I83" s="0">
-        <v>0.57735026918962573</v>
+        <v>2.6575364531836625</v>
       </c>
       <c r="J83" s="0">
-        <v>11.25</v>
+        <v>20.75</v>
       </c>
       <c r="K83" s="0">
-        <v>3.7052890125692848</v>
+        <v>8.1687922403906601</v>
       </c>
       <c r="L83" s="0">
-        <v>19</v>
+        <v>22.5</v>
       </c>
       <c r="M83" s="0">
-        <v>3.7638632635454048</v>
+        <v>4.1932485418030412</v>
       </c>
       <c r="N83" s="0">
-        <v>180.63086507936512</v>
+        <v>347.29934920634918</v>
       </c>
       <c r="O83" s="0">
-        <v>56.827780897825768</v>
+        <v>158.54349546179873</v>
       </c>
       <c r="P83" s="0">
-        <v>33.331271553867516</v>
+        <v>61.087244108135195</v>
       </c>
       <c r="Q83" s="0">
-        <v>10.908418051016014</v>
+        <v>23.644092541978718</v>
       </c>
     </row>
     <row r="84">
@@ -4543,46 +4543,46 @@
         <v>7</v>
       </c>
       <c r="D84" s="0">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E84" s="0">
         <v>4</v>
       </c>
       <c r="F84" s="0">
+        <v>22.75</v>
+      </c>
+      <c r="G84" s="0">
+        <v>7.9621500446382782</v>
+      </c>
+      <c r="H84" s="0">
+        <v>3.75</v>
+      </c>
+      <c r="I84" s="0">
+        <v>1.6520189667999174</v>
+      </c>
+      <c r="J84" s="0">
         <v>20.25</v>
       </c>
-      <c r="G84" s="0">
-        <v>4.3851073723076235</v>
-      </c>
-      <c r="H84" s="0">
-        <v>6.25</v>
-      </c>
-      <c r="I84" s="0">
-        <v>0.8539125638299665</v>
-      </c>
-      <c r="J84" s="0">
-        <v>14.75</v>
-      </c>
       <c r="K84" s="0">
-        <v>3.4247870980057527</v>
+        <v>7.2154348448309058</v>
       </c>
       <c r="L84" s="0">
-        <v>28.25</v>
+        <v>22.75</v>
       </c>
       <c r="M84" s="0">
-        <v>3.2755406678389241</v>
+        <v>7.9201746613737418</v>
       </c>
       <c r="N84" s="0">
-        <v>37.815684210526243</v>
+        <v>708.12724358974367</v>
       </c>
       <c r="O84" s="0">
-        <v>1.8994763552843577</v>
+        <v>561.21766446431354</v>
       </c>
       <c r="P84" s="0">
-        <v>42.385652341041457</v>
+        <v>59.918759272660409</v>
       </c>
       <c r="Q84" s="0">
-        <v>9.7041622791667983</v>
+        <v>21.035766353192841</v>
       </c>
     </row>
     <row r="85">
@@ -4596,46 +4596,46 @@
         <v>7</v>
       </c>
       <c r="D85" s="0">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E85" s="0">
         <v>4</v>
       </c>
       <c r="F85" s="0">
-        <v>16.25</v>
+        <v>33.25</v>
       </c>
       <c r="G85" s="0">
-        <v>6.472699076377129</v>
+        <v>5.1051444641655346</v>
       </c>
       <c r="H85" s="0">
-        <v>2.25</v>
+        <v>7.5</v>
       </c>
       <c r="I85" s="0">
-        <v>0.75</v>
+        <v>2.5331140255951108</v>
       </c>
       <c r="J85" s="0">
-        <v>13.25</v>
+        <v>25.75</v>
       </c>
       <c r="K85" s="0">
-        <v>6.0190669265814503</v>
+        <v>3.6371921404658658</v>
       </c>
       <c r="L85" s="0">
-        <v>38</v>
+        <v>24.25</v>
       </c>
       <c r="M85" s="0">
-        <v>10.230672835481871</v>
+        <v>4.7147817199385456</v>
       </c>
       <c r="N85" s="0">
-        <v>192.07601190476191</v>
+        <v>142.98126893939397</v>
       </c>
       <c r="O85" s="0">
-        <v>142.6828567917467</v>
+        <v>36.959966323550475</v>
       </c>
       <c r="P85" s="0">
-        <v>37.897737798460241</v>
+        <v>75.952174842019758</v>
       </c>
       <c r="Q85" s="0">
-        <v>17.144928103836946</v>
+        <v>10.026028158088602</v>
       </c>
     </row>
     <row r="86">
@@ -4649,46 +4649,46 @@
         <v>7</v>
       </c>
       <c r="D86" s="0">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E86" s="0">
         <v>4</v>
       </c>
       <c r="F86" s="0">
-        <v>22.25</v>
+        <v>17.25</v>
       </c>
       <c r="G86" s="0">
-        <v>7.6634957210575037</v>
+        <v>4.732423621500228</v>
       </c>
       <c r="H86" s="0">
-        <v>3</v>
+        <v>9.25</v>
       </c>
       <c r="I86" s="0">
-        <v>0.40824829046386302</v>
+        <v>6.9686799323831767</v>
       </c>
       <c r="J86" s="0">
-        <v>19</v>
+        <v>14.25</v>
       </c>
       <c r="K86" s="0">
-        <v>6.8920243760451108</v>
+        <v>4.4040700872412701</v>
       </c>
       <c r="L86" s="0">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="M86" s="0">
-        <v>21.459263733874934</v>
+        <v>18.605554726120548</v>
       </c>
       <c r="N86" s="0">
-        <v>615.06807878151267</v>
+        <v>306.30527777777775</v>
       </c>
       <c r="O86" s="0">
-        <v>460.5257697598081</v>
+        <v>144.64282161794904</v>
       </c>
       <c r="P86" s="0">
-        <v>54.455336742364189</v>
+        <v>42.255216679264713</v>
       </c>
       <c r="Q86" s="0">
-        <v>19.576332030120021</v>
+        <v>13.15467278835462</v>
       </c>
     </row>
     <row r="87">
@@ -4702,46 +4702,46 @@
         <v>7</v>
       </c>
       <c r="D87" s="0">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E87" s="0">
         <v>4</v>
       </c>
       <c r="F87" s="0">
-        <v>21</v>
+        <v>16.25</v>
       </c>
       <c r="G87" s="0">
-        <v>8.755950357709132</v>
+        <v>5.5733742024019888</v>
       </c>
       <c r="H87" s="0">
-        <v>2.75</v>
+        <v>1</v>
       </c>
       <c r="I87" s="0">
-        <v>0.62915286960589578</v>
+        <v>0.57735026918962573</v>
       </c>
       <c r="J87" s="0">
-        <v>17.25</v>
+        <v>11.25</v>
       </c>
       <c r="K87" s="0">
-        <v>7.8885465496925775</v>
+        <v>3.7052890125692848</v>
       </c>
       <c r="L87" s="0">
-        <v>53.75</v>
+        <v>19</v>
       </c>
       <c r="M87" s="0">
-        <v>23.792068005955262</v>
+        <v>3.7638632635454048</v>
       </c>
       <c r="N87" s="0">
-        <v>112.15200541795659</v>
+        <v>180.63086507936512</v>
       </c>
       <c r="O87" s="0">
-        <v>71.500120010883265</v>
+        <v>56.827780897825768</v>
       </c>
       <c r="P87" s="0">
-        <v>49.359967524618412</v>
+        <v>33.331271553867516</v>
       </c>
       <c r="Q87" s="0">
-        <v>22.448608149749454</v>
+        <v>10.908418051016014</v>
       </c>
     </row>
     <row r="88">
@@ -4755,46 +4755,46 @@
         <v>7</v>
       </c>
       <c r="D88" s="0">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E88" s="0">
         <v>4</v>
       </c>
       <c r="F88" s="0">
-        <v>26</v>
+        <v>20.25</v>
       </c>
       <c r="G88" s="0">
-        <v>13.310396938734272</v>
+        <v>4.3851073723076235</v>
       </c>
       <c r="H88" s="0">
-        <v>3.75</v>
+        <v>6.25</v>
       </c>
       <c r="I88" s="0">
-        <v>1.4930394055974097</v>
+        <v>0.8539125638299665</v>
       </c>
       <c r="J88" s="0">
-        <v>18.5</v>
+        <v>14.75</v>
       </c>
       <c r="K88" s="0">
-        <v>8.9116029235298999</v>
+        <v>3.4247870980057527</v>
       </c>
       <c r="L88" s="0">
-        <v>43.25</v>
+        <v>28.25</v>
       </c>
       <c r="M88" s="0">
-        <v>16.064323826417343</v>
+        <v>3.2755406678389241</v>
       </c>
       <c r="N88" s="0">
-        <v>28.478772522522533</v>
+        <v>37.815684210526243</v>
       </c>
       <c r="O88" s="0">
-        <v>12.265467204347953</v>
+        <v>1.8994763552843577</v>
       </c>
       <c r="P88" s="0">
-        <v>52.883651201847584</v>
+        <v>42.385652341041457</v>
       </c>
       <c r="Q88" s="0">
-        <v>25.424951259661405</v>
+        <v>9.7041622791667983</v>
       </c>
     </row>
     <row r="89">
@@ -4808,46 +4808,46 @@
         <v>7</v>
       </c>
       <c r="D89" s="0">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E89" s="0">
         <v>4</v>
       </c>
       <c r="F89" s="0">
-        <v>39.25</v>
+        <v>16.25</v>
       </c>
       <c r="G89" s="0">
-        <v>17.556456552125393</v>
+        <v>6.472699076377129</v>
       </c>
       <c r="H89" s="0">
-        <v>8.25</v>
+        <v>2.25</v>
       </c>
       <c r="I89" s="0">
-        <v>3.8378596465564847</v>
+        <v>0.75</v>
       </c>
       <c r="J89" s="0">
-        <v>0</v>
+        <v>13.25</v>
       </c>
       <c r="K89" s="0">
-        <v>0</v>
+        <v>6.0190669265814503</v>
       </c>
       <c r="L89" s="0">
-        <v>42.5</v>
+        <v>38</v>
       </c>
       <c r="M89" s="0">
-        <v>13.979151142564653</v>
+        <v>10.230672835481871</v>
       </c>
       <c r="N89" s="0">
-        <v>291.79665170940166</v>
+        <v>192.07601190476191</v>
       </c>
       <c r="O89" s="0">
-        <v>112.60182057523238</v>
+        <v>142.6828567917467</v>
       </c>
       <c r="P89" s="0">
-        <v>0</v>
+        <v>37.897737798460241</v>
       </c>
       <c r="Q89" s="0">
-        <v>0</v>
+        <v>17.144928103836946</v>
       </c>
     </row>
     <row r="90">
@@ -4861,46 +4861,46 @@
         <v>7</v>
       </c>
       <c r="D90" s="0">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E90" s="0">
         <v>4</v>
       </c>
       <c r="F90" s="0">
-        <v>18.5</v>
+        <v>22.25</v>
       </c>
       <c r="G90" s="0">
-        <v>8.6071675557835707</v>
+        <v>7.6634957210575037</v>
       </c>
       <c r="H90" s="0">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="I90" s="0">
-        <v>3.7638632635454048</v>
+        <v>0.40824829046386302</v>
       </c>
       <c r="J90" s="0">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="K90" s="0">
-        <v>0</v>
+        <v>6.8920243760451108</v>
       </c>
       <c r="L90" s="0">
-        <v>16.25</v>
+        <v>55</v>
       </c>
       <c r="M90" s="0">
-        <v>3.5207716957129347</v>
+        <v>21.459263733874934</v>
       </c>
       <c r="N90" s="0">
-        <v>81.147666666666623</v>
+        <v>615.06807878151267</v>
       </c>
       <c r="O90" s="0">
-        <v>42.923520281663414</v>
+        <v>460.5257697598081</v>
       </c>
       <c r="P90" s="0">
-        <v>0</v>
+        <v>54.455336742364189</v>
       </c>
       <c r="Q90" s="0">
-        <v>0</v>
+        <v>19.576332030120021</v>
       </c>
     </row>
     <row r="91">
@@ -4914,46 +4914,46 @@
         <v>7</v>
       </c>
       <c r="D91" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E91" s="0">
         <v>4</v>
       </c>
       <c r="F91" s="0">
-        <v>14.25</v>
+        <v>21</v>
       </c>
       <c r="G91" s="0">
-        <v>5.2181574014844232</v>
+        <v>8.755950357709132</v>
       </c>
       <c r="H91" s="0">
-        <v>6.25</v>
+        <v>2.75</v>
       </c>
       <c r="I91" s="0">
-        <v>2.5617376914898995</v>
+        <v>0.62915286960589578</v>
       </c>
       <c r="J91" s="0">
-        <v>0</v>
+        <v>17.25</v>
       </c>
       <c r="K91" s="0">
-        <v>0</v>
+        <v>7.8885465496925775</v>
       </c>
       <c r="L91" s="0">
-        <v>9.25</v>
+        <v>53.75</v>
       </c>
       <c r="M91" s="0">
-        <v>2.75</v>
+        <v>23.792068005955262</v>
       </c>
       <c r="N91" s="0">
-        <v>156.85175925925927</v>
+        <v>112.15200541795659</v>
       </c>
       <c r="O91" s="0">
-        <v>66.038910817667698</v>
+        <v>71.500120010883265</v>
       </c>
       <c r="P91" s="0">
-        <v>0</v>
+        <v>49.359967524618412</v>
       </c>
       <c r="Q91" s="0">
-        <v>0</v>
+        <v>22.448608149749454</v>
       </c>
     </row>
     <row r="92">
@@ -4967,46 +4967,46 @@
         <v>7</v>
       </c>
       <c r="D92" s="0">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E92" s="0">
         <v>4</v>
       </c>
       <c r="F92" s="0">
-        <v>25.75</v>
+        <v>26</v>
       </c>
       <c r="G92" s="0">
-        <v>10.201102881551583</v>
+        <v>13.310396938734272</v>
       </c>
       <c r="H92" s="0">
-        <v>10</v>
+        <v>3.75</v>
       </c>
       <c r="I92" s="0">
-        <v>3.5118845842842465</v>
+        <v>1.4930394055974097</v>
       </c>
       <c r="J92" s="0">
-        <v>0</v>
+        <v>18.5</v>
       </c>
       <c r="K92" s="0">
-        <v>0</v>
+        <v>8.9116029235298999</v>
       </c>
       <c r="L92" s="0">
-        <v>13</v>
+        <v>43.25</v>
       </c>
       <c r="M92" s="0">
-        <v>2.4152294576982398</v>
+        <v>16.064323826417343</v>
       </c>
       <c r="N92" s="0">
-        <v>321.09545238095239</v>
+        <v>28.478772522522533</v>
       </c>
       <c r="O92" s="0">
-        <v>123.04154441678047</v>
+        <v>12.265467204347953</v>
       </c>
       <c r="P92" s="0">
-        <v>0</v>
+        <v>52.883651201847584</v>
       </c>
       <c r="Q92" s="0">
-        <v>0</v>
+        <v>25.424951259661405</v>
       </c>
     </row>
     <row r="93">
@@ -5020,22 +5020,22 @@
         <v>7</v>
       </c>
       <c r="D93" s="0">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E93" s="0">
         <v>4</v>
       </c>
       <c r="F93" s="0">
-        <v>13.25</v>
+        <v>39.25</v>
       </c>
       <c r="G93" s="0">
-        <v>4.3277207241995947</v>
+        <v>17.556456552125393</v>
       </c>
       <c r="H93" s="0">
-        <v>10.5</v>
+        <v>8.25</v>
       </c>
       <c r="I93" s="0">
-        <v>6.0346223300772239</v>
+        <v>3.8378596465564847</v>
       </c>
       <c r="J93" s="0">
         <v>0</v>
@@ -5044,16 +5044,16 @@
         <v>0</v>
       </c>
       <c r="L93" s="0">
-        <v>10</v>
+        <v>42.5</v>
       </c>
       <c r="M93" s="0">
-        <v>1.4719601443879744</v>
+        <v>13.979151142564653</v>
       </c>
       <c r="N93" s="0">
-        <v>65.152738095238107</v>
+        <v>291.79665170940166</v>
       </c>
       <c r="O93" s="0">
-        <v>34.843507789493984</v>
+        <v>112.60182057523238</v>
       </c>
       <c r="P93" s="0">
         <v>0</v>
@@ -5073,22 +5073,22 @@
         <v>7</v>
       </c>
       <c r="D94" s="0">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E94" s="0">
         <v>4</v>
       </c>
       <c r="F94" s="0">
-        <v>9</v>
+        <v>18.5</v>
       </c>
       <c r="G94" s="0">
-        <v>4.377975178854566</v>
+        <v>8.6071675557835707</v>
       </c>
       <c r="H94" s="0">
-        <v>8.25</v>
+        <v>11</v>
       </c>
       <c r="I94" s="0">
-        <v>3.4490336810958131</v>
+        <v>3.7638632635454048</v>
       </c>
       <c r="J94" s="0">
         <v>0</v>
@@ -5097,16 +5097,16 @@
         <v>0</v>
       </c>
       <c r="L94" s="0">
-        <v>10.25</v>
+        <v>16.25</v>
       </c>
       <c r="M94" s="0">
-        <v>3.3509948771471834</v>
+        <v>3.5207716957129347</v>
       </c>
       <c r="N94" s="0">
-        <v>640.75212499999998</v>
+        <v>81.147666666666623</v>
       </c>
       <c r="O94" s="0">
-        <v>435.16586522116165</v>
+        <v>42.923520281663414</v>
       </c>
       <c r="P94" s="0">
         <v>0</v>
@@ -5126,45 +5126,363 @@
         <v>7</v>
       </c>
       <c r="D95" s="0">
+        <v>18</v>
+      </c>
+      <c r="E95" s="0">
+        <v>4</v>
+      </c>
+      <c r="F95" s="0">
+        <v>14.25</v>
+      </c>
+      <c r="G95" s="0">
+        <v>5.2181574014844232</v>
+      </c>
+      <c r="H95" s="0">
+        <v>6.25</v>
+      </c>
+      <c r="I95" s="0">
+        <v>2.5617376914898995</v>
+      </c>
+      <c r="J95" s="0">
+        <v>0</v>
+      </c>
+      <c r="K95" s="0">
+        <v>0</v>
+      </c>
+      <c r="L95" s="0">
+        <v>9.25</v>
+      </c>
+      <c r="M95" s="0">
+        <v>2.75</v>
+      </c>
+      <c r="N95" s="0">
+        <v>156.85175925925927</v>
+      </c>
+      <c r="O95" s="0">
+        <v>66.038910817667698</v>
+      </c>
+      <c r="P95" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q95" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C96" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D96" s="0">
+        <v>19</v>
+      </c>
+      <c r="E96" s="0">
+        <v>4</v>
+      </c>
+      <c r="F96" s="0">
+        <v>16</v>
+      </c>
+      <c r="G96" s="0">
+        <v>3.3416562759605704</v>
+      </c>
+      <c r="H96" s="0">
+        <v>7.5</v>
+      </c>
+      <c r="I96" s="0">
+        <v>3.5707142142714252</v>
+      </c>
+      <c r="J96" s="0">
+        <v>0</v>
+      </c>
+      <c r="K96" s="0">
+        <v>0</v>
+      </c>
+      <c r="L96" s="0">
+        <v>9.5</v>
+      </c>
+      <c r="M96" s="0">
+        <v>2.8722813232690143</v>
+      </c>
+      <c r="N96" s="0">
+        <v>489.71300000000025</v>
+      </c>
+      <c r="O96" s="0">
+        <v>131.99411073604765</v>
+      </c>
+      <c r="P96" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q96" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C97" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D97" s="0">
+        <v>20</v>
+      </c>
+      <c r="E97" s="0">
+        <v>4</v>
+      </c>
+      <c r="F97" s="0">
+        <v>9.75</v>
+      </c>
+      <c r="G97" s="0">
+        <v>5.5733742024019888</v>
+      </c>
+      <c r="H97" s="0">
+        <v>10.25</v>
+      </c>
+      <c r="I97" s="0">
+        <v>4.2695628191498329</v>
+      </c>
+      <c r="J97" s="0">
+        <v>0</v>
+      </c>
+      <c r="K97" s="0">
+        <v>0</v>
+      </c>
+      <c r="L97" s="0">
+        <v>9.75</v>
+      </c>
+      <c r="M97" s="0">
+        <v>3.7052890125692848</v>
+      </c>
+      <c r="N97" s="0">
+        <v>654.82050000000027</v>
+      </c>
+      <c r="O97" s="0">
+        <v>622.29343778565055</v>
+      </c>
+      <c r="P97" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q97" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98" s="0">
+        <v>21</v>
+      </c>
+      <c r="E98" s="0">
+        <v>4</v>
+      </c>
+      <c r="F98" s="0">
+        <v>25.75</v>
+      </c>
+      <c r="G98" s="0">
+        <v>10.201102881551583</v>
+      </c>
+      <c r="H98" s="0">
+        <v>10</v>
+      </c>
+      <c r="I98" s="0">
+        <v>3.5118845842842465</v>
+      </c>
+      <c r="J98" s="0">
+        <v>0</v>
+      </c>
+      <c r="K98" s="0">
+        <v>0</v>
+      </c>
+      <c r="L98" s="0">
+        <v>13</v>
+      </c>
+      <c r="M98" s="0">
+        <v>2.4152294576982398</v>
+      </c>
+      <c r="N98" s="0">
+        <v>321.09545238095239</v>
+      </c>
+      <c r="O98" s="0">
+        <v>123.04154441678047</v>
+      </c>
+      <c r="P98" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q98" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C99" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D99" s="0">
+        <v>22</v>
+      </c>
+      <c r="E99" s="0">
+        <v>4</v>
+      </c>
+      <c r="F99" s="0">
+        <v>13.25</v>
+      </c>
+      <c r="G99" s="0">
+        <v>4.3277207241995947</v>
+      </c>
+      <c r="H99" s="0">
+        <v>10.5</v>
+      </c>
+      <c r="I99" s="0">
+        <v>6.0346223300772239</v>
+      </c>
+      <c r="J99" s="0">
+        <v>0</v>
+      </c>
+      <c r="K99" s="0">
+        <v>0</v>
+      </c>
+      <c r="L99" s="0">
+        <v>10</v>
+      </c>
+      <c r="M99" s="0">
+        <v>1.4719601443879744</v>
+      </c>
+      <c r="N99" s="0">
+        <v>65.152738095238107</v>
+      </c>
+      <c r="O99" s="0">
+        <v>34.843507789493984</v>
+      </c>
+      <c r="P99" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q99" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C100" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D100" s="0">
+        <v>23</v>
+      </c>
+      <c r="E100" s="0">
+        <v>4</v>
+      </c>
+      <c r="F100" s="0">
+        <v>9</v>
+      </c>
+      <c r="G100" s="0">
+        <v>4.377975178854566</v>
+      </c>
+      <c r="H100" s="0">
+        <v>8.25</v>
+      </c>
+      <c r="I100" s="0">
+        <v>3.4490336810958131</v>
+      </c>
+      <c r="J100" s="0">
+        <v>0</v>
+      </c>
+      <c r="K100" s="0">
+        <v>0</v>
+      </c>
+      <c r="L100" s="0">
+        <v>10.25</v>
+      </c>
+      <c r="M100" s="0">
+        <v>3.3509948771471834</v>
+      </c>
+      <c r="N100" s="0">
+        <v>640.75212499999998</v>
+      </c>
+      <c r="O100" s="0">
+        <v>435.16586522116165</v>
+      </c>
+      <c r="P100" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q100" s="0">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C101" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D101" s="0">
         <v>24</v>
       </c>
-      <c r="E95" s="0">
-        <v>4</v>
-      </c>
-      <c r="F95" s="0">
+      <c r="E101" s="0">
+        <v>4</v>
+      </c>
+      <c r="F101" s="0">
         <v>14.5</v>
       </c>
-      <c r="G95" s="0">
+      <c r="G101" s="0">
         <v>5.315072906367325</v>
       </c>
-      <c r="H95" s="0">
+      <c r="H101" s="0">
         <v>3</v>
       </c>
-      <c r="I95" s="0">
+      <c r="I101" s="0">
         <v>1.0801234497346435</v>
       </c>
-      <c r="J95" s="0">
+      <c r="J101" s="0">
         <v>7.75</v>
       </c>
-      <c r="K95" s="0">
+      <c r="K101" s="0">
         <v>2.7801378862687129</v>
       </c>
-      <c r="L95" s="0">
+      <c r="L101" s="0">
         <v>8</v>
       </c>
-      <c r="M95" s="0">
+      <c r="M101" s="0">
         <v>3.7638632635454048</v>
       </c>
-      <c r="N95" s="0">
+      <c r="N101" s="0">
         <v>8.0465824915824893</v>
       </c>
-      <c r="O95" s="0">
+      <c r="O101" s="0">
         <v>4.0773943075567818</v>
       </c>
-      <c r="P95" s="0">
-        <v>0</v>
-      </c>
-      <c r="Q95" s="0">
+      <c r="P101" s="0">
+        <v>0</v>
+      </c>
+      <c r="Q101" s="0">
         <v>0</v>
       </c>
     </row>

</xml_diff>